<commit_message>
Updated test cases and bug metrics
Tested the application and updated the Iteration 1 Test Cases document.
Added the bugs into the bug metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>S/N</t>
   </si>
@@ -105,6 +105,81 @@
   </si>
   <si>
     <t>The system does not need immediate fixing, could be fixed during buffer time or during coding sessions</t>
+  </si>
+  <si>
+    <t>Login/ Logout (Student)</t>
+  </si>
+  <si>
+    <t>User is still able to access the application after logging out</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>viewNurseHomePage.jsp</t>
+  </si>
+  <si>
+    <t>Unsolved</t>
+  </si>
+  <si>
+    <t>Create Student</t>
+  </si>
+  <si>
+    <t>No success message shown when account is created successfully</t>
+  </si>
+  <si>
+    <t>Create Lecturer</t>
+  </si>
+  <si>
+    <t>Create Admin</t>
+  </si>
+  <si>
+    <t>Edit Student Account</t>
+  </si>
+  <si>
+    <t>No success message when  student account is created successfully</t>
+  </si>
+  <si>
+    <t>No success message when  lecturer account is created successfully</t>
+  </si>
+  <si>
+    <t>No success message when  admin account is created successfully</t>
+  </si>
+  <si>
+    <t>Edit Lecturer Account</t>
+  </si>
+  <si>
+    <t>Edit Admin Account</t>
+  </si>
+  <si>
+    <t>Delete Student Account</t>
+  </si>
+  <si>
+    <t>No success message when student account is deleted succssfully</t>
+  </si>
+  <si>
+    <t>Delete Lecturer Account</t>
+  </si>
+  <si>
+    <t>Delete Admin Account</t>
+  </si>
+  <si>
+    <t>No success message when Lecturer account is deleted succssfully</t>
+  </si>
+  <si>
+    <t>No success message when admin account is deleted succssfully</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>viewAdminAccounts.jsp</t>
+  </si>
+  <si>
+    <t>viewLecturerAccounts.jsp</t>
+  </si>
+  <si>
+    <t>viewNurseAccounts.jsp</t>
   </si>
 </sst>
 </file>
@@ -287,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -303,6 +378,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -313,29 +407,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -643,23 +726,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="4.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="31" style="2" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
@@ -669,57 +752,63 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="12"/>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="19">
+        <f>SUM(G8:G17)</f>
+        <v>14</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="G4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -753,122 +842,295 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+    <row r="8" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+    <row r="9" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+    <row r="10" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+    <row r="11" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+    <row r="12" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+    <row r="13" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+    <row r="14" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="9">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+    <row r="15" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="9">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+    <row r="16" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="9">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="18">
+        <v>41913</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -878,6 +1140,7 @@
     <mergeCell ref="B2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -886,7 +1149,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,13 +1169,13 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -960,19 +1223,19 @@
     </row>
     <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="19">
+      <c r="B8" s="13">
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">

</xml_diff>

<commit_message>
Updated bug metrics after debugging
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>S/N</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>viewNurseAccounts.jsp</t>
+  </si>
+  <si>
+    <t>Included a protect.jsp in viewNurseHomePage.jsp to prevent user from viewing page after log out</t>
+  </si>
+  <si>
+    <t>Wei Yi</t>
+  </si>
+  <si>
+    <t>04/10/2014</t>
   </si>
 </sst>
 </file>
@@ -397,6 +406,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,20 +424,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -728,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -752,60 +761,60 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="19">
+      <c r="C4" s="21"/>
+      <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
       </c>
-      <c r="E4" s="20"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -842,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9">
         <v>1</v>
       </c>
@@ -855,7 +864,7 @@
       <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="14">
         <v>41913</v>
       </c>
       <c r="G8" s="5">
@@ -867,9 +876,15 @@
       <c r="I8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
@@ -884,7 +899,7 @@
       <c r="E9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="14">
         <v>41913</v>
       </c>
       <c r="G9" s="5">
@@ -896,9 +911,16 @@
       <c r="I9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="J9" s="5" t="str">
+        <f>CONCATENATE("Stored success message as an attribute and displayed it on ",D9)</f>
+        <v>Stored success message as an attribute and displayed it on viewNurseAccounts.jsp</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
@@ -913,7 +935,7 @@
       <c r="E10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="14">
         <v>41913</v>
       </c>
       <c r="G10" s="5">
@@ -925,9 +947,16 @@
       <c r="I10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="J10" s="5" t="str">
+        <f>CONCATENATE("Stored success message as an attribute and displayed it on ",D10)</f>
+        <v>Stored success message as an attribute and displayed it on viewLecturerAccounts.jsp</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9">
@@ -942,7 +971,7 @@
       <c r="E11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="14">
         <v>41913</v>
       </c>
       <c r="G11" s="5">
@@ -954,9 +983,16 @@
       <c r="I11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="5" t="str">
+        <f t="shared" ref="J11:J17" si="0">CONCATENATE("Stored success message as an attribute and displayed it on ",D11)</f>
+        <v>Stored success message as an attribute and displayed it on viewAdminAccounts.jsp</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
@@ -971,7 +1007,7 @@
       <c r="E12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="14">
         <v>41913</v>
       </c>
       <c r="G12" s="5">
@@ -983,9 +1019,16 @@
       <c r="I12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="J12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewNurseAccounts.jsp</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
@@ -1000,7 +1043,7 @@
       <c r="E13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="14">
         <v>41913</v>
       </c>
       <c r="G13" s="5">
@@ -1012,9 +1055,16 @@
       <c r="I13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="J13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewLecturerAccounts.jsp</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="9">
@@ -1029,7 +1079,7 @@
       <c r="E14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="14">
         <v>41913</v>
       </c>
       <c r="G14" s="5">
@@ -1041,9 +1091,16 @@
       <c r="I14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="J14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewAdminAccounts.jsp</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="9">
@@ -1058,7 +1115,7 @@
       <c r="E15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="14">
         <v>41913</v>
       </c>
       <c r="G15" s="5">
@@ -1070,9 +1127,16 @@
       <c r="I15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="J15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewNurseAccounts.jsp</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="9">
@@ -1087,7 +1151,7 @@
       <c r="E16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="14">
         <v>41913</v>
       </c>
       <c r="G16" s="5">
@@ -1099,9 +1163,16 @@
       <c r="I16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="J16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewLecturerAccounts.jsp</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="9">
@@ -1116,7 +1187,7 @@
       <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="14">
         <v>41913</v>
       </c>
       <c r="G17" s="5">
@@ -1128,9 +1199,16 @@
       <c r="I17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="J17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stored success message as an attribute and displayed it on viewAdminAccounts.jsp</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Debugged bug 1 and 3
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
   <si>
     <t>S/N</t>
   </si>
@@ -213,9 +213,6 @@
     <t>User is prompted an a message saying “Activating this case would deactivate other cases”</t>
   </si>
   <si>
-    <t>017-10-2014</t>
-  </si>
-  <si>
     <t>Unsolved</t>
   </si>
   <si>
@@ -226,6 +223,15 @@
   </si>
   <si>
     <t>No success message when case is deleted</t>
+  </si>
+  <si>
+    <t>Shi Qi</t>
+  </si>
+  <si>
+    <t>Changed the textbox in editPracticalGroupAccount to dropdown to eliminate error of typing the lecturer ID that does not exist</t>
+  </si>
+  <si>
+    <t>Displayed success message. Previously, the success message was set, but was not displayed on viewScenarioAdmin</t>
   </si>
 </sst>
 </file>
@@ -455,6 +461,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -469,9 +478,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -804,28 +810,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -834,30 +840,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1269,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1293,28 +1299,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1323,30 +1329,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1383,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9">
         <v>1</v>
       </c>
@@ -1396,8 +1402,8 @@
       <c r="E8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>65</v>
+      <c r="F8" s="14">
+        <v>41929</v>
       </c>
       <c r="G8" s="5">
         <v>5</v>
@@ -1407,11 +1413,17 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="14">
+        <v>41931</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
@@ -1437,24 +1449,24 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F10" s="14">
         <v>41930</v>
@@ -1467,11 +1479,17 @@
         <v>Low Impact</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="14">
+        <v>41931</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11"/>
@@ -1646,7 +1664,7 @@
     </row>
     <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="23">
+      <c r="B4" s="18">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">

</xml_diff>

<commit_message>
Resolved bug 2 and updated bug metrics
Renamed one method; retrieveActivatedScenario instead of
retrieveActivatedStatus
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>S/N</t>
   </si>
@@ -213,9 +213,6 @@
     <t>User is prompted an a message saying “Activating this case would deactivate other cases”</t>
   </si>
   <si>
-    <t>Unsolved</t>
-  </si>
-  <si>
     <t>Delete Case Scenario (Admin)</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Displayed success message. Previously, the success message was set, but was not displayed on viewScenarioAdmin</t>
+  </si>
+  <si>
+    <t>Use a text message on the page instead of a pop up to warn user about activating one case will deactivate the other case.</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1276,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1416,10 +1416,10 @@
         <v>57</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L8" s="14">
         <v>41931</v>
@@ -1449,24 +1449,30 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="14">
+        <v>41931</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="F10" s="14">
         <v>41930</v>
@@ -1482,10 +1488,10 @@
         <v>57</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10" s="14">
         <v>41931</v>

</xml_diff>

<commit_message>
Updated bug metrics of iteration 3
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" activeTab="2"/>
@@ -12,12 +12,12 @@
     <sheet name="Iteration 3" sheetId="6" r:id="rId3"/>
     <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
   <si>
     <t>S/N</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>Last updated time for despatching report is incorrect</t>
+  </si>
+  <si>
+    <t>Hui Ping (Grace)</t>
+  </si>
+  <si>
+    <t>Debugged it by changing request to sesion and invalid the session only when the student submits not saved</t>
+  </si>
+  <si>
+    <t>Added if else statement to check group names and/or condition if multidisciplinary notes is empty, and set error message accordingly</t>
   </si>
 </sst>
 </file>
@@ -614,6 +623,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,15 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -703,7 +712,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,7 +747,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -973,28 +982,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1003,30 +1012,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1439,7 +1448,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1462,28 +1471,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1492,30 +1501,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1812,29 +1821,29 @@
   <sheetData>
     <row r="1" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="19"/>
     </row>
     <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="23"/>
     </row>
     <row r="4" spans="2:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="24">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -1843,28 +1852,28 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="19"/>
     </row>
     <row r="7" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1902,7 +1911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="29">
         <v>1</v>
       </c>
@@ -1928,15 +1937,21 @@
       <c r="I8" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
+      <c r="J8" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="33">
+        <v>41942</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="26">
         <v>2</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="37" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="27" t="s">
@@ -1958,18 +1973,24 @@
       <c r="I9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
+      <c r="J9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="33">
+        <v>41940</v>
+      </c>
     </row>
     <row r="10" spans="2:13" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="26">
         <v>3</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="36" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="27" t="s">

</xml_diff>

<commit_message>
Updated bug metrics for iteration 3
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" activeTab="2"/>
@@ -12,12 +12,12 @@
     <sheet name="Iteration 3" sheetId="6" r:id="rId3"/>
     <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
   <si>
     <t>S/N</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Saved multidisciplinary notes is blank after doing other tasks (update vital signs)</t>
   </si>
   <si>
-    <t>Unsolved</t>
-  </si>
-  <si>
     <t>View Patient's investigation reports</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>Added if else statement to check group names and/or condition if multidisciplinary notes is empty, and set error message accordingly</t>
+  </si>
+  <si>
+    <t>Set timezone in pages where datetime is formatted.</t>
   </si>
 </sst>
 </file>
@@ -712,7 +712,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,7 +747,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1797,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1938,10 +1938,10 @@
         <v>57</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L8" s="33">
         <v>41942</v>
@@ -1974,10 +1974,10 @@
         <v>57</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L9" s="33">
         <v>41940</v>
@@ -1988,29 +1988,35 @@
         <v>3</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="28">
         <v>41945</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="32">
         <v>5</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28"/>
+      <c r="I10" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="33">
+        <v>41945</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="21"/>

</xml_diff>

<commit_message>
Updated metrics for iteration 3
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="83">
   <si>
     <t>S/N</t>
   </si>
@@ -528,7 +528,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,9 +578,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -646,9 +643,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -982,28 +976,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1012,30 +1006,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1448,7 +1442,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1471,28 +1465,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1501,30 +1495,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1795,98 +1789,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M17"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="4.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="23" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="23" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="23" customWidth="1"/>
-    <col min="10" max="10" width="31" style="23" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="23" customWidth="1"/>
-    <col min="12" max="12" width="14" style="23" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="23" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="4.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="22" customWidth="1"/>
+    <col min="10" max="10" width="31" style="22" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="14" style="22" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="22" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="23"/>
-    </row>
-    <row r="4" spans="2:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="43" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="24">
+      <c r="C4" s="42"/>
+      <c r="D4" s="23">
         <f>SUM(G8:G10)</f>
         <v>15</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-    </row>
-    <row r="5" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="39" t="s">
+      <c r="G4" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+    </row>
+    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="20" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
+    </row>
+    <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1911,224 +1905,224 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="29">
+    <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="28">
         <v>1</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>41939</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>5</v>
       </c>
-      <c r="H8" s="32" t="str">
+      <c r="H8" s="31" t="str">
         <f>VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2)</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="32">
         <v>41942</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="26">
+    <row r="9" spans="2:12" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="25">
         <v>2</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>41939</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>5</v>
       </c>
-      <c r="H9" s="32" t="str">
+      <c r="H9" s="31" t="str">
         <f>VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2)</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="32">
         <v>41940</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="26">
+    <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="25">
         <v>3</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>41945</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>5</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="32">
         <v>41945</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="str">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21" t="str">
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20" t="str">
         <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21" t="str">
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21" t="str">
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21" t="str">
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="str">
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20" t="str">
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21" t="str">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20" t="str">
         <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Debugged for iteration 4
Updated Bug Metrics.
Added a new method to only update lecturer ID for modification to
practical group's lecturer-in-charge.
Made changes to alignments on create, edit accounts page.
Standardized all successful/error messages notification.
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="87">
   <si>
     <t>S/N</t>
   </si>
@@ -275,10 +275,10 @@
     <t>http://hsemr-wpinapp.rhcloud.com/hsemr/editPracticalGroupAccount.jsp</t>
   </si>
   <si>
-    <t>user is able to save even if password field is blank</t>
-  </si>
-  <si>
-    <t>Unsolved</t>
+    <t>when user only wants to modify lecturer, they are not required to fill up password. However, database is updated with empty password if password field is left empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added new method to only update lecturer ID if user only wants to update lecturer-in-charge. </t>
   </si>
 </sst>
 </file>
@@ -730,6 +730,45 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,45 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1116,28 +1116,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1146,30 +1146,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1605,28 +1605,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1635,30 +1635,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1932,7 +1932,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1955,28 +1955,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="22"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="23">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -1985,30 +1985,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
@@ -2283,7 +2283,7 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:L8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2306,28 +2306,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="22"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="23">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2336,33 +2336,33 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
@@ -2396,8 +2396,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47">
+    <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="42">
         <v>1</v>
       </c>
       <c r="C8" s="33" t="s">
@@ -2409,48 +2409,54 @@
       <c r="E8" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="39">
         <v>41957</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="40">
         <v>5</v>
       </c>
-      <c r="H8" s="45" t="str">
+      <c r="H8" s="40" t="str">
         <f>VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2)</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="48"/>
+      <c r="K8" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="32">
+        <v>41959</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="33"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="48"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="43"/>
     </row>
     <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="49"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>

</xml_diff>

<commit_message>
Updated metrics for Iteration 4
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>S/N</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">Added new method to only update lecturer ID if user only wants to update lecturer-in-charge. </t>
+  </si>
+  <si>
+    <t>Iteration 4 (3 November 2014 - 15 November 2014)</t>
   </si>
 </sst>
 </file>
@@ -371,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -477,21 +480,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -506,116 +494,8 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -629,7 +509,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,9 +559,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -694,80 +571,53 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,6 +633,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1116,28 +990,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1146,30 +1020,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1605,28 +1479,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1635,30 +1509,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1932,133 +1806,133 @@
   <dimension ref="B1:L17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B7" sqref="B7:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="4.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="22" customWidth="1"/>
-    <col min="10" max="10" width="31" style="22" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="14" style="22" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="22" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.140625" style="21"/>
+    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="31" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="14" style="21" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="23">
+      <c r="C4" s="45"/>
+      <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="28">
+      <c r="B8" s="24">
         <v>1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="36">
         <v>41939</v>
       </c>
       <c r="G8" s="31">
@@ -2077,24 +1951,24 @@
       <c r="K8" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="36">
         <v>41942</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>2</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="37" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="36">
         <v>41939</v>
       </c>
       <c r="G9" s="31">
@@ -2113,24 +1987,24 @@
       <c r="K9" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="32">
+      <c r="L9" s="36">
         <v>41940</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>3</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="40">
         <v>41945</v>
       </c>
       <c r="G10" s="31">
@@ -2148,121 +2022,121 @@
       <c r="K10" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="36">
         <v>41945</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20" t="str">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20" t="str">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="str">
         <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20" t="str">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20" t="str">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20" t="str">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20" t="str">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19" t="str">
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20" t="str">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="str">
         <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2280,295 +2154,337 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="4.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="22" customWidth="1"/>
-    <col min="10" max="10" width="31" style="22" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="14" style="22" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="22" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.140625" style="21"/>
+    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="31" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="14" style="21" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
-    </row>
-    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22"/>
-    </row>
-    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="48"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="21"/>
+    </row>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="23">
+      <c r="C4" s="50"/>
+      <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-    </row>
-    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-    </row>
-    <row r="7" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="53"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="48"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="42">
+    <row r="8" spans="1:17" ht="120.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="25">
         <v>1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="32">
         <v>41957</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="30">
         <v>5</v>
       </c>
-      <c r="H8" s="40" t="str">
+      <c r="H8" s="30" t="str">
         <f>VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2)</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="36">
         <v>41959</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="42"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="43"/>
-    </row>
-    <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="50"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20" t="str">
+    <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20" t="str">
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="str">
         <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20" t="str">
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20" t="str">
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20" t="str">
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20" t="str">
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19" t="str">
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20" t="str">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="str">
         <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2586,7 +2502,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new test case for iteration 5
Tested all test cases and updated bug metrics.
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
     <sheet name="Iteration 2" sheetId="5" r:id="rId2"/>
     <sheet name="Iteration 3" sheetId="6" r:id="rId3"/>
     <sheet name="Iteration 4" sheetId="7" r:id="rId4"/>
-    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId5"/>
+    <sheet name="Iteration 5" sheetId="8" r:id="rId5"/>
+    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
   <si>
     <t>S/N</t>
   </si>
@@ -282,6 +283,21 @@
   </si>
   <si>
     <t>Iteration 4 (3 November 2014 - 15 November 2014)</t>
+  </si>
+  <si>
+    <t>Iteration 5 (15 December 2014 - 28 December 2014)</t>
+  </si>
+  <si>
+    <t>State transition</t>
+  </si>
+  <si>
+    <t>editStateLecturer.jsp</t>
+  </si>
+  <si>
+    <t>Null pointer found when no scenario is activated</t>
+  </si>
+  <si>
+    <t>Unsolved</t>
   </si>
 </sst>
 </file>
@@ -509,7 +525,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -618,6 +634,9 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,28 +1009,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1020,30 +1039,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1479,28 +1498,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1509,30 +1528,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1829,28 +1848,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -1859,30 +1878,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -2156,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2180,28 +2199,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2210,30 +2229,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -2498,6 +2517,343 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="21"/>
+    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="31" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="14" style="21" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="49"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="21"/>
+    </row>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="22">
+        <f>SUM(G8:G10)</f>
+        <v>5</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="54"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="25">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="32">
+        <v>41998</v>
+      </c>
+      <c r="G8" s="30">
+        <v>5</v>
+      </c>
+      <c r="H8" s="30" t="str">
+        <f>VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2)</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="str">
+        <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="B6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Debugged for iteration 5
Added if else to catch the null pointer exception to show a message.
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="94">
   <si>
     <t>S/N</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Unsolved</t>
+  </si>
+  <si>
+    <t>Added a if else statement to catch the null pointer to show a message</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:L10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2176,7 +2179,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2230,7 +2233,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -2520,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2574,7 +2577,9 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="52" t="s">
+        <v>23</v>
+      </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="53"/>
@@ -2632,7 +2637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="25">
         <v>1</v>
       </c>
@@ -2658,9 +2663,15 @@
       <c r="I8" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
+      <c r="J8" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="36">
+        <v>41970</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
@@ -2858,7 +2869,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Debugged for iteration 5"
This reverts commit f957c41bbcd1a757429f3c4786aa1eda182b946d.
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
   <si>
     <t>S/N</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Unsolved</t>
-  </si>
-  <si>
-    <t>Added a if else statement to catch the null pointer to show a message</t>
   </si>
 </sst>
 </file>
@@ -1827,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2179,7 +2176,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:L4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2233,7 +2230,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -2523,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:L4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2577,9 +2574,7 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="52" t="s">
-        <v>23</v>
-      </c>
+      <c r="G4" s="52"/>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="53"/>
@@ -2637,7 +2632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="25">
         <v>1</v>
       </c>
@@ -2663,15 +2658,9 @@
       <c r="I8" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J8" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="36">
-        <v>41970</v>
-      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
@@ -2869,7 +2858,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tested app and found new bugs
Added bugs into bug metrics and updated test cases
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="101">
   <si>
     <t>S/N</t>
   </si>
@@ -301,6 +301,27 @@
   </si>
   <si>
     <t>Added if else statement to catch the null pointer to show a error message</t>
+  </si>
+  <si>
+    <t>Temperature Charts</t>
+  </si>
+  <si>
+    <t>viewPatientInformation.jsp</t>
+  </si>
+  <si>
+    <t>Date and time stated is wrong</t>
+  </si>
+  <si>
+    <t>Respiratory Rate Chart</t>
+  </si>
+  <si>
+    <t>Heart Rate Chart</t>
+  </si>
+  <si>
+    <t>Blood Pressure Chart</t>
+  </si>
+  <si>
+    <t>SPO Chart</t>
   </si>
 </sst>
 </file>
@@ -528,7 +549,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2524,7 +2548,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2570,8 +2594,8 @@
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="22">
-        <f>SUM(G8:G10)</f>
-        <v>5</v>
+        <f>SUM(G8:G116)</f>
+        <v>30</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="7" t="s">
@@ -2638,7 +2662,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25">
+      <c r="B8" s="55">
         <v>1</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -2673,104 +2697,175 @@
         <v>42001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="B9" s="28">
+        <v>2</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="32">
+        <v>42001</v>
+      </c>
+      <c r="G9" s="30">
+        <v>5</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
     </row>
-    <row r="10" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="B10" s="28">
+        <v>3</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="32">
+        <v>42001</v>
+      </c>
+      <c r="G10" s="30">
+        <v>5</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19" t="str">
-        <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="B11" s="28">
+        <v>4</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="32">
+        <v>42001</v>
+      </c>
+      <c r="G11" s="30">
+        <v>5</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19" t="str">
-        <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="B12" s="28">
+        <v>5</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="32">
+        <v>42001</v>
+      </c>
+      <c r="G12" s="30">
+        <v>5</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19" t="str">
-        <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="B13" s="28">
+        <v>6</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="32">
+        <v>42001</v>
+      </c>
+      <c r="G13" s="30">
+        <v>5</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>

</xml_diff>

<commit_message>
Debugged and Updated Bug Metric
Display dates as String on chart to avoid conversion error on different
platforms (IE, Chrome, Openshift)
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="102">
   <si>
     <t>S/N</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>SPO Chart</t>
+  </si>
+  <si>
+    <t>Printed the dates of vital signs as String on chart instead of Date to avoid conversion error at different platforms</t>
   </si>
 </sst>
 </file>
@@ -662,6 +665,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -700,9 +706,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1036,28 +1039,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1066,30 +1069,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1525,28 +1528,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1555,30 +1558,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1875,28 +1878,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -1905,30 +1908,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -2226,28 +2229,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2256,30 +2259,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -2548,7 +2551,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2571,28 +2574,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -2601,30 +2604,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -2662,7 +2665,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="55">
+      <c r="B8" s="42">
         <v>1</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -2723,9 +2726,15 @@
       <c r="I9" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="J9" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="36">
+        <v>42002</v>
+      </c>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
@@ -2758,16 +2767,22 @@
       <c r="I10" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
+      <c r="J10" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="36">
+        <v>42002</v>
+      </c>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="28">
         <v>4</v>
@@ -2793,16 +2808,22 @@
       <c r="I11" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
+      <c r="J11" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="36">
+        <v>42002</v>
+      </c>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="28">
         <v>5</v>
@@ -2828,16 +2849,22 @@
       <c r="I12" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
+      <c r="J12" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="36">
+        <v>42002</v>
+      </c>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="28">
         <v>6</v>
@@ -2863,9 +2890,15 @@
       <c r="I13" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
+      <c r="J13" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" s="36">
+        <v>42002</v>
+      </c>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>

</xml_diff>

<commit_message>
Solved bug 1 and updated bug metrics
Added required to the scenario so that it will validate when it is empty
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="115">
   <si>
     <t>S/N</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">Beds displayed are different from the scenarios </t>
+  </si>
+  <si>
+    <t>Added required in the input text for scenario</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -705,8 +708,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,12 +765,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -766,18 +778,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1092,48 +1092,48 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="2" customWidth="1"/>
     <col min="10" max="10" width="31" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="13" max="13" width="14.7265625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+    <row r="1" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-    </row>
-    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+    </row>
+    <row r="3" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1142,32 +1142,32 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-    </row>
-    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+    </row>
+    <row r="5" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
-    </row>
-    <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>1</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>2</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>3</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>4</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>5</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>6</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>7</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>8</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>9</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>10</v>
       </c>
@@ -1581,48 +1581,48 @@
       <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="2"/>
+    <col min="2" max="2" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="2" customWidth="1"/>
     <col min="10" max="10" width="31" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="13" max="13" width="14.7265625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+    <row r="1" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-    </row>
-    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+    </row>
+    <row r="3" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1631,32 +1631,32 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-    </row>
-    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+    </row>
+    <row r="5" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
-    </row>
-    <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>0</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="63" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>1</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>2</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>3</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
@@ -1815,7 +1815,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -1831,7 +1831,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -1847,7 +1847,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -1863,7 +1863,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
@@ -1879,7 +1879,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -1895,7 +1895,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -1931,48 +1931,48 @@
       <selection activeCell="B7" sqref="B7:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="21"/>
+    <col min="2" max="2" width="4.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="21" customWidth="1"/>
     <col min="10" max="10" width="31" style="21" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="21" customWidth="1"/>
     <col min="12" max="12" width="14" style="21" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="13" width="14.7265625" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+    <row r="1" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-    </row>
-    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+    </row>
+    <row r="3" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21"/>
     </row>
-    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -1981,32 +1981,32 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-    </row>
-    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+    </row>
+    <row r="5" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
-    </row>
-    <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="24">
         <v>1</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>41942</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24">
         <v>2</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>41940</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24">
         <v>3</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>41945</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -2164,7 +2164,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -2180,7 +2180,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -2196,7 +2196,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -2212,7 +2212,7 @@
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -2228,7 +2228,7 @@
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2244,7 +2244,7 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -2279,51 +2279,51 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="21"/>
+    <col min="2" max="2" width="4.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="21" customWidth="1"/>
     <col min="10" max="10" width="31" style="21" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="21" customWidth="1"/>
     <col min="12" max="12" width="14" style="21" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="13" width="14.7265625" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+    <row r="1" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+    </row>
+    <row r="3" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21"/>
     </row>
-    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51" t="s">
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2332,32 +2332,32 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
+    </row>
+    <row r="5" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>0</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="120.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="102" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>1</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>41959</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -2447,7 +2447,7 @@
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
     </row>
-    <row r="10" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -2466,7 +2466,7 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -2488,7 +2488,7 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -2510,7 +2510,7 @@
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -2532,7 +2532,7 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -2554,7 +2554,7 @@
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -2576,7 +2576,7 @@
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2592,7 +2592,7 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -2623,52 +2623,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="B8:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="21"/>
+    <col min="2" max="2" width="4.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="21" customWidth="1"/>
     <col min="10" max="10" width="31" style="21" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="21" customWidth="1"/>
     <col min="12" max="12" width="14" style="21" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="21"/>
+    <col min="13" max="13" width="14.7265625" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+    <row r="1" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
+    </row>
+    <row r="3" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21"/>
     </row>
-    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51" t="s">
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -2677,32 +2677,32 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
+    </row>
+    <row r="5" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="41" t="s">
         <v>0</v>
       </c>
@@ -2737,17 +2737,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="42">
+    <row r="8" spans="1:17" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="32">
         <v>1</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="32" t="s">
         <v>91</v>
       </c>
       <c r="F8" s="32">
@@ -2773,15 +2773,15 @@
         <v>42001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
-      <c r="B9" s="28">
+      <c r="B9" s="32">
         <v>2</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -2814,15 +2814,15 @@
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
     </row>
-    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19"/>
-      <c r="B10" s="28">
+      <c r="B10" s="32">
         <v>3</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E10" s="32" t="s">
@@ -2855,15 +2855,15 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="19"/>
-      <c r="B11" s="28">
+      <c r="B11" s="32">
         <v>4</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="32" t="s">
@@ -2896,15 +2896,15 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19"/>
-      <c r="B12" s="28">
+      <c r="B12" s="32">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E12" s="32" t="s">
@@ -2937,15 +2937,15 @@
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
     </row>
-    <row r="13" spans="1:17" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="19"/>
-      <c r="B13" s="28">
+      <c r="B13" s="32">
         <v>6</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E13" s="32" t="s">
@@ -2978,7 +2978,7 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -3000,7 +3000,7 @@
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -3022,7 +3022,7 @@
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -3038,7 +3038,7 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -3069,82 +3069,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="57"/>
-    <col min="2" max="2" width="4.42578125" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="57" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" style="57" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="57" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="57" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="57" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="57" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="57" customWidth="1"/>
-    <col min="10" max="10" width="31" style="57" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="57" customWidth="1"/>
-    <col min="12" max="12" width="14" style="57" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="57" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="9.1796875" style="43"/>
+    <col min="2" max="2" width="4.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="43" customWidth="1"/>
+    <col min="4" max="4" width="42.54296875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="43" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="43" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="43" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="31" style="43" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="43" customWidth="1"/>
+    <col min="12" max="12" width="14" style="43" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" style="43" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="58" t="s">
+    <row r="1" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="60"/>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
+    </row>
+    <row r="3" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63">
+      <c r="C4" s="65"/>
+      <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>25</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="58" t="s">
+      <c r="G4" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
+    </row>
+    <row r="5" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="63"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="34" t="s">
         <v>0</v>
       </c>
@@ -3179,17 +3181,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="30">
         <v>1</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="32" t="s">
         <v>111</v>
       </c>
       <c r="F8" s="32">
@@ -3202,20 +3204,28 @@
         <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:17" ht="120.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="65"/>
+      <c r="I8" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="36">
+        <v>42014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="46"/>
       <c r="B9" s="28">
         <v>2</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="42" t="s">
         <v>104</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -3235,21 +3245,21 @@
       <c r="J9" s="35"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-    </row>
-    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+    </row>
+    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="46"/>
       <c r="B10" s="28">
         <v>3</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="32" t="s">
@@ -3269,21 +3279,21 @@
       <c r="J10" s="35"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-    </row>
-    <row r="11" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="65"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+    </row>
+    <row r="11" spans="1:17" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="46"/>
       <c r="B11" s="28">
         <v>4</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E11" s="32" t="s">
@@ -3303,21 +3313,21 @@
       <c r="J11" s="35"/>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-    </row>
-    <row r="12" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="65"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+    </row>
+    <row r="12" spans="1:17" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="46"/>
       <c r="B12" s="28">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E12" s="32" t="s">
@@ -3337,14 +3347,14 @@
       <c r="J12" s="35"/>
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-    </row>
-    <row r="13" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="65"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="46"/>
       <c r="B13" s="28"/>
       <c r="C13" s="26"/>
       <c r="D13" s="29"/>
@@ -3359,87 +3369,87 @@
       <c r="J13" s="35"/>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65" t="str">
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+    </row>
+    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="65"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65" t="str">
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65" t="str">
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46" t="str">
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65" t="str">
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+    </row>
+    <row r="17" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46" t="str">
         <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3464,25 +3474,25 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="13.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="94" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="11" t="s">
         <v>13</v>
@@ -3494,7 +3504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -3506,7 +3516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="18">
         <v>5</v>
@@ -3518,7 +3528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="4">
         <v>10</v>
@@ -3530,13 +3540,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
       <c r="B7" s="11" t="s">
         <v>7</v>
@@ -3548,7 +3558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="13">
         <v>0</v>
@@ -3560,7 +3570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="4">
         <v>5</v>
@@ -3572,7 +3582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="4">
         <v>10</v>
@@ -3584,19 +3594,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>

</xml_diff>

<commit_message>
Testing for iteration 6
All test cases passed
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="117">
   <si>
     <t>S/N</t>
   </si>
@@ -326,9 +326,6 @@
   </si>
   <si>
     <t>Printed the dates of vital signs as String on chart instead of Date to avoid conversion error at different platforms</t>
-  </si>
-  <si>
-    <t>Iteration 6 (15 December 2014 - 28 December 2014)</t>
   </si>
   <si>
     <t>View Ward Information</t>
@@ -346,16 +343,10 @@
     <t>Create Scenario</t>
   </si>
   <si>
-    <t>Documents &amp; Investigations</t>
-  </si>
-  <si>
     <t>SPO Charts</t>
   </si>
   <si>
     <t>Data does not match the time</t>
-  </si>
-  <si>
-    <t>30 seconds timer does not work</t>
   </si>
   <si>
     <t>Scenario created when scenario name is empty</t>
@@ -381,6 +372,9 @@
   <si>
     <t xml:space="preserve">Added a new method in ScenarioDAO to sort the beds in ASC order
  </t>
+  </si>
+  <si>
+    <t>Iteration 6 (5 Janurary 2015- 11 Janurary 2015)</t>
   </si>
 </sst>
 </file>
@@ -608,7 +602,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -791,6 +785,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3082,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3107,7 +3119,7 @@
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="61" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C2" s="62"/>
       <c r="D2" s="62"/>
@@ -3128,7 +3140,7 @@
       <c r="C4" s="65"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="7" t="s">
@@ -3146,7 +3158,7 @@
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="61" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -3199,13 +3211,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F8" s="32">
         <v>42013</v>
@@ -3221,7 +3233,7 @@
         <v>57</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K8" s="35" t="s">
         <v>68</v>
@@ -3236,13 +3248,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>104</v>
-      </c>
       <c r="E9" s="32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F9" s="32">
         <v>42013</v>
@@ -3258,10 +3270,10 @@
         <v>57</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L9" s="36">
         <v>42014</v>
@@ -3278,13 +3290,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F10" s="32">
         <v>42013</v>
@@ -3296,10 +3308,18 @@
         <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
+      <c r="I10" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="36">
+        <v>42014</v>
+      </c>
       <c r="M10" s="46"/>
       <c r="N10" s="46"/>
       <c r="O10" s="46"/>
@@ -3308,19 +3328,19 @@
     </row>
     <row r="11" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="46"/>
-      <c r="B11" s="28">
+      <c r="B11" s="30">
         <v>4</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="32">
+      <c r="E11" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="30">
         <v>42013</v>
       </c>
       <c r="G11" s="30">
@@ -3330,14 +3350,14 @@
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>116</v>
+      <c r="J11" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="L11" s="36">
         <v>42014</v>
@@ -3348,64 +3368,41 @@
       <c r="P11" s="46"/>
       <c r="Q11" s="46"/>
     </row>
-    <row r="12" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="46"/>
-      <c r="B12" s="28">
-        <v>5</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="32">
-        <v>42013</v>
-      </c>
-      <c r="G12" s="30">
-        <v>5</v>
-      </c>
-      <c r="H12" s="30" t="str">
-        <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v xml:space="preserve">High Impact </v>
-      </c>
-      <c r="I12" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" s="36">
-        <v>42014</v>
-      </c>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
       <c r="P12" s="46"/>
       <c r="Q12" s="46"/>
     </row>
-    <row r="13" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30" t="str">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="46"/>
       <c r="N13" s="46"/>
       <c r="O13" s="46"/>
@@ -3500,7 +3497,6 @@
     <hyperlink ref="D8" r:id="rId2"/>
     <hyperlink ref="D10" r:id="rId3"/>
     <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D12" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated documentations - minutes
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -733,6 +733,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -785,24 +803,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1137,28 +1137,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1167,30 +1167,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1626,28 +1626,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1656,30 +1656,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1976,28 +1976,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -2006,30 +2006,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -2327,28 +2327,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2357,30 +2357,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="60"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -2648,8 +2648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="B8:D13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2672,28 +2672,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -2702,30 +2702,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="60"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -3094,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3118,26 +3118,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="69"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="65"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -3146,30 +3146,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="60"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="63"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="69"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -3334,7 +3334,7 @@
       <c r="C11" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="53" t="s">
         <v>74</v>
       </c>
       <c r="E11" s="30" t="s">
@@ -3370,17 +3370,17 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="46"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
@@ -3389,20 +3389,20 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69" t="str">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
       <c r="M13" s="46"/>
       <c r="N13" s="46"/>
       <c r="O13" s="46"/>

</xml_diff>

<commit_message>
Testing for iteration 7
Added new test cases for iteration 7
Updated bug metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -13,14 +13,16 @@
     <sheet name="Iteration 4" sheetId="7" r:id="rId4"/>
     <sheet name="Iteration 5" sheetId="8" r:id="rId5"/>
     <sheet name="Iteration 6" sheetId="9" r:id="rId6"/>
-    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId7"/>
+    <sheet name="Iteration 7" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId8"/>
+    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="149">
   <si>
     <t>S/N</t>
   </si>
@@ -375,13 +377,109 @@
   </si>
   <si>
     <t>Iteration 6 (5 Janurary 2015- 11 Janurary 2015)</t>
+  </si>
+  <si>
+    <t>Reset case</t>
+  </si>
+  <si>
+    <t>http://localhost:8084/hsemr/viewPatientInformation.jsp</t>
+  </si>
+  <si>
+    <t>Vital signs are not deleted after clicking reset </t>
+  </si>
+  <si>
+    <t>Medical history not deleted after clicking reset</t>
+  </si>
+  <si>
+    <t>View Activated Case Scenario</t>
+  </si>
+  <si>
+    <t>http://localhost:8084/hsemr/viewWardInformation.jsp</t>
+  </si>
+  <si>
+    <t>Error message should be displayed when no case is activated</t>
+  </si>
+  <si>
+    <t>unsolved</t>
+  </si>
+  <si>
+    <t>Case Setup - State V2</t>
+  </si>
+  <si>
+    <t>http://localhost:8084/hsemr/createScenario.jsp</t>
+  </si>
+  <si>
+    <t>No error message for case name</t>
+  </si>
+  <si>
+    <t>No error message for gender selection</t>
+  </si>
+  <si>
+    <t>taken down hr,bp,intake, output, administer medicine</t>
+  </si>
+  <si>
+    <t>xuanqi, linwei, qiwei, linxuan, qiping</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t> Edit</t>
+  </si>
+  <si>
+    <t> Copy</t>
+  </si>
+  <si>
+    <t> Delete</t>
+  </si>
+  <si>
+    <t>testestest</t>
+  </si>
+  <si>
+    <t>tingting, shiqi, weiyi, gladys, jocelyn, grace</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>Administered panadol at 5.34pm</t>
+  </si>
+  <si>
+    <t>glad, sq, wy, grace, joce</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>Chemistry report despatched. Blood pressure, spo2, respiration rate, heart rate normal.</t>
+  </si>
+  <si>
+    <t>a, b, c, d</t>
+  </si>
+  <si>
+    <t>Hi hi 5 nov</t>
+  </si>
+  <si>
+    <t>grace Test</t>
+  </si>
+  <si>
+    <t>SC4</t>
+  </si>
+  <si>
+    <t>Activate Case</t>
+  </si>
+  <si>
+    <t>Null pointer in student portal when admin activate case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,8 +538,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +584,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFDFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -596,13 +726,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBBBBBB"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -751,6 +910,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,6 +966,99 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="11" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -822,6 +1077,695 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Edit">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3657600" y="3200400"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Copy">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4267200" y="3200400"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Delete">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4876800" y="3200400"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Edit">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3657600" y="4171950"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Copy">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4267200" y="4171950"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Delete">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4876800" y="4171950"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Edit">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3657600" y="4981575"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Copy">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4267200" y="4981575"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Delete">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4876800" y="4981575"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Edit">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3657600" y="6600825"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="Copy">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4267200" y="6600825"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Delete">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4876800" y="6600825"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1137,28 +2081,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -1167,30 +2111,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1626,28 +2570,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -1656,30 +2600,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -1976,28 +2920,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -2006,30 +2950,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -2327,28 +3271,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -2357,30 +3301,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="62"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -2672,28 +3616,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -2702,30 +3646,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="62"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -3094,8 +4038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3118,26 +4062,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -3146,30 +4090,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="70"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -3503,6 +4447,646 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="43"/>
+    <col min="2" max="2" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="43" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="43" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="43" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="43" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="43" customWidth="1"/>
+    <col min="10" max="10" width="31" style="43" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="14" style="43" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="43" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="44">
+        <f>SUM(G8:G116)</f>
+        <v>18</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="67"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="70"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="30">
+        <v>1</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="32">
+        <v>42024</v>
+      </c>
+      <c r="G8" s="30">
+        <v>5</v>
+      </c>
+      <c r="H8" s="30" t="str">
+        <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="28">
+        <v>2</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="32">
+        <v>42024</v>
+      </c>
+      <c r="G9" s="30">
+        <v>5</v>
+      </c>
+      <c r="H9" s="30" t="str">
+        <f>IFERROR(VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+    </row>
+    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46"/>
+      <c r="B10" s="28">
+        <v>3</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="32">
+        <v>42024</v>
+      </c>
+      <c r="G10" s="30">
+        <v>1</v>
+      </c>
+      <c r="H10" s="74" t="str">
+        <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+    </row>
+    <row r="11" spans="1:17" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46"/>
+      <c r="B11" s="30">
+        <v>4</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="36">
+        <v>42024</v>
+      </c>
+      <c r="G11" s="31">
+        <v>1</v>
+      </c>
+      <c r="H11" s="83" t="str">
+        <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+    </row>
+    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46"/>
+      <c r="B12" s="26">
+        <v>5</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="36">
+        <v>42024</v>
+      </c>
+      <c r="G12" s="31">
+        <v>1</v>
+      </c>
+      <c r="H12" s="35" t="str">
+        <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" s="80"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+    </row>
+    <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="101"/>
+      <c r="B13" s="102">
+        <v>6</v>
+      </c>
+      <c r="C13" s="102" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="103" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="36">
+        <v>42024</v>
+      </c>
+      <c r="G13" s="78">
+        <v>5</v>
+      </c>
+      <c r="H13" s="76" t="str">
+        <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I13" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="84"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="46"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H18" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G18,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H19" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G19,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H20" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G20,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G21,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H22" s="49"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H23" s="49"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H24" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="B6:L6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="F11:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
+      <c r="F11" s="86">
+        <v>1</v>
+      </c>
+      <c r="K11" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" s="87" t="s">
+        <v>130</v>
+      </c>
+      <c r="M11" s="88">
+        <v>41929.583333333336</v>
+      </c>
+      <c r="N11" s="89" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="89" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="90"/>
+      <c r="G12" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="92">
+        <v>2</v>
+      </c>
+      <c r="K12" s="93" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" s="93" t="s">
+        <v>137</v>
+      </c>
+      <c r="M12" s="94">
+        <v>41933.475694444445</v>
+      </c>
+      <c r="N12" s="95" t="s">
+        <v>138</v>
+      </c>
+      <c r="O12" s="95" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="96"/>
+      <c r="G13" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="97" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" s="98">
+        <v>3</v>
+      </c>
+      <c r="K13" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="99" t="s">
+        <v>140</v>
+      </c>
+      <c r="M13" s="100">
+        <v>41939.449386574073</v>
+      </c>
+      <c r="N13" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="O13" s="89" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="F14" s="90"/>
+      <c r="G14" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="92">
+        <v>4</v>
+      </c>
+      <c r="K14" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="L14" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="94">
+        <v>41941.431875000002</v>
+      </c>
+      <c r="N14" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="O14" s="95" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F15" s="96"/>
+      <c r="G15" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="97" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" s="98">
+        <v>5</v>
+      </c>
+      <c r="K15" s="99" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" s="99" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="100">
+        <v>41948.662094907406</v>
+      </c>
+      <c r="N15" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="O15" s="89" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N11" r:id="rId1" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P02%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O11" r:id="rId2" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G12" r:id="rId3" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H12" r:id="rId4" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I12" r:id="rId5" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+2&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N12" r:id="rId6" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P03%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O12" r:id="rId7" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G13" r:id="rId8" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H13" r:id="rId9" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I13" r:id="rId10" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+3&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N13" r:id="rId11" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O13" r:id="rId12" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G14" r:id="rId13" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H14" r:id="rId14" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I14" r:id="rId15" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+4&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N14" r:id="rId16" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O14" r:id="rId17" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G15" r:id="rId18" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H15" r:id="rId19" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I15" r:id="rId20" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+5&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N15" r:id="rId21" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O15" r:id="rId22" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC4%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId23"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>

<commit_message>
solved route and frequency
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="150">
   <si>
     <t>S/N</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Null pointer in student portal when admin activate case</t>
+  </si>
+  <si>
+    <t>Added required for case name</t>
   </si>
 </sst>
 </file>
@@ -913,6 +916,99 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="11" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -966,99 +1062,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="11" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2081,28 +2084,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2111,30 +2114,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2570,28 +2573,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2600,30 +2603,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2920,28 +2923,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="88"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -2950,30 +2953,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3271,28 +3274,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="93"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3301,30 +3304,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="67"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="62"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="93"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3616,28 +3619,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="62"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="93"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3646,30 +3649,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="67"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="62"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="93"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4062,26 +4065,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="70"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="101"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="72"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4090,30 +4093,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="67"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="70"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4451,7 +4454,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4474,26 +4477,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="70"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="101"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="72"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>18</v>
@@ -4502,30 +4505,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="67"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="70"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="54" t="s">
@@ -4572,7 +4575,7 @@
       <c r="D8" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="55" t="s">
         <v>119</v>
       </c>
       <c r="F8" s="32">
@@ -4639,7 +4642,7 @@
       <c r="D10" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="81" t="s">
+      <c r="E10" s="63" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="32">
@@ -4648,7 +4651,7 @@
       <c r="G10" s="30">
         <v>1</v>
       </c>
-      <c r="H10" s="74" t="str">
+      <c r="H10" s="56" t="str">
         <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
@@ -4684,16 +4687,22 @@
       <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="83" t="str">
+      <c r="H11" s="65" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="85"/>
+        <v>57</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="67">
+        <v>42026</v>
+      </c>
       <c r="M11" s="46"/>
       <c r="N11" s="46"/>
       <c r="O11" s="46"/>
@@ -4727,8 +4736,8 @@
       <c r="I12" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="80"/>
-      <c r="L12" s="79"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="61"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
@@ -4736,46 +4745,46 @@
       <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="101"/>
-      <c r="B13" s="102">
+      <c r="A13" s="83"/>
+      <c r="B13" s="84">
         <v>6</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="64" t="s">
         <v>148</v>
       </c>
       <c r="F13" s="36">
         <v>42024</v>
       </c>
-      <c r="G13" s="78">
+      <c r="G13" s="60">
         <v>5</v>
       </c>
-      <c r="H13" s="76" t="str">
+      <c r="H13" s="58" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="84"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="101"/>
-      <c r="O13" s="101"/>
-      <c r="P13" s="101"/>
-      <c r="Q13" s="101"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="83"/>
+      <c r="P13" s="83"/>
+      <c r="Q13" s="83"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="46"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="46"/>
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
@@ -4917,142 +4926,142 @@
   </cols>
   <sheetData>
     <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="86">
+      <c r="F11" s="68">
         <v>1</v>
       </c>
-      <c r="K11" s="87" t="s">
+      <c r="K11" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="87" t="s">
+      <c r="L11" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="88">
+      <c r="M11" s="70">
         <v>41929.583333333336</v>
       </c>
-      <c r="N11" s="89" t="s">
+      <c r="N11" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="89" t="s">
+      <c r="O11" s="71" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="90"/>
-      <c r="G12" s="91" t="s">
+      <c r="F12" s="72"/>
+      <c r="G12" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="91" t="s">
+      <c r="H12" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="91" t="s">
+      <c r="I12" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="92">
+      <c r="J12" s="74">
         <v>2</v>
       </c>
-      <c r="K12" s="93" t="s">
+      <c r="K12" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="93" t="s">
+      <c r="L12" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="94">
+      <c r="M12" s="76">
         <v>41933.475694444445</v>
       </c>
-      <c r="N12" s="95" t="s">
+      <c r="N12" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="95" t="s">
+      <c r="O12" s="77" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="96"/>
-      <c r="G13" s="97" t="s">
+      <c r="F13" s="78"/>
+      <c r="G13" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="97" t="s">
+      <c r="H13" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="97" t="s">
+      <c r="I13" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="J13" s="98">
+      <c r="J13" s="80">
         <v>3</v>
       </c>
-      <c r="K13" s="99" t="s">
+      <c r="K13" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="L13" s="99" t="s">
+      <c r="L13" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="M13" s="100">
+      <c r="M13" s="82">
         <v>41939.449386574073</v>
       </c>
-      <c r="N13" s="89" t="s">
+      <c r="N13" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="O13" s="89" t="s">
+      <c r="O13" s="71" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="90"/>
-      <c r="G14" s="91" t="s">
+      <c r="F14" s="72"/>
+      <c r="G14" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="91" t="s">
+      <c r="H14" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="91" t="s">
+      <c r="I14" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="92">
+      <c r="J14" s="74">
         <v>4</v>
       </c>
-      <c r="K14" s="93" t="s">
+      <c r="K14" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="93" t="s">
+      <c r="L14" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="94">
+      <c r="M14" s="76">
         <v>41941.431875000002</v>
       </c>
-      <c r="N14" s="95" t="s">
+      <c r="N14" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="O14" s="95" t="s">
+      <c r="O14" s="77" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="96"/>
-      <c r="G15" s="97" t="s">
+      <c r="F15" s="78"/>
+      <c r="G15" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="97" t="s">
+      <c r="H15" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="I15" s="97" t="s">
+      <c r="I15" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="98">
+      <c r="J15" s="80">
         <v>5</v>
       </c>
-      <c r="K15" s="99" t="s">
+      <c r="K15" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="100">
+      <c r="M15" s="82">
         <v>41948.662094907406</v>
       </c>
-      <c r="N15" s="89" t="s">
+      <c r="N15" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="89" t="s">
+      <c r="O15" s="71" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated bug metrics with new bugs
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="154">
   <si>
     <t>S/N</t>
   </si>
@@ -476,13 +476,25 @@
   </si>
   <si>
     <t>Added required for case name</t>
+  </si>
+  <si>
+    <t>Case setup</t>
+  </si>
+  <si>
+    <t>http://hsemr-wpinapp.rhcloud.com/hsemr/createMedicationBC.jsp</t>
+  </si>
+  <si>
+    <t>Unable to click frequency drop down list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to click Route drop down list </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,14 +549,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -764,7 +768,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -922,9 +926,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -955,6 +956,42 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="10" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -964,42 +1001,6 @@
     <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="11" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1062,6 +1063,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2084,28 +2109,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="90"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2114,30 +2139,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="87"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2573,28 +2598,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="90"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2603,30 +2628,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="87"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2923,28 +2948,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="90"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -2953,30 +2978,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="87"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3274,28 +3299,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="93"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="92"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="95"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3304,30 +3329,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="98"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="93"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="92"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3619,28 +3644,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="93"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="92"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="95"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3649,30 +3674,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="98"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="93"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="92"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4065,26 +4090,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4093,30 +4118,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="98"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="100"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4454,7 +4479,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B6" sqref="B6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4477,58 +4502,58 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="98"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="100"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="54" t="s">
@@ -4642,7 +4667,7 @@
       <c r="D10" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="62" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="32">
@@ -4687,20 +4712,20 @@
       <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="65" t="str">
+      <c r="H11" s="64" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="K11" s="67" t="s">
+      <c r="K11" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="67">
+      <c r="L11" s="66">
         <v>42026</v>
       </c>
       <c r="M11" s="46"/>
@@ -4736,8 +4761,8 @@
       <c r="I12" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="62"/>
-      <c r="L12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
@@ -4745,84 +4770,108 @@
       <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84">
+      <c r="A13" s="82"/>
+      <c r="B13" s="83">
         <v>6</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="63" t="s">
         <v>148</v>
       </c>
       <c r="F13" s="36">
         <v>42024</v>
       </c>
-      <c r="G13" s="60">
+      <c r="G13" s="59">
         <v>5</v>
       </c>
-      <c r="H13" s="58" t="str">
+      <c r="H13" s="57" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I13" s="60" t="s">
+      <c r="I13" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="66"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="51" t="str">
+      <c r="J13" s="65"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+    </row>
+    <row r="14" spans="1:17" s="103" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="104"/>
+      <c r="B14" s="105">
+        <v>7</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="105" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="110">
+        <v>42025</v>
+      </c>
+      <c r="G14" s="105">
+        <v>1</v>
+      </c>
+      <c r="H14" s="57" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="51" t="str">
+        <v>Low Impact</v>
+      </c>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+    </row>
+    <row r="15" spans="1:17" s="103" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="104"/>
+      <c r="B15" s="107">
+        <v>8</v>
+      </c>
+      <c r="C15" s="105" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="109" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="107" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="110">
+        <v>42025</v>
+      </c>
+      <c r="G15" s="107">
+        <v>1</v>
+      </c>
+      <c r="H15" s="59" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
+        <v>Low Impact</v>
+      </c>
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="104"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="46"/>
@@ -4898,8 +4947,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1"/>
+    <hyperlink ref="D14" r:id="rId2"/>
+    <hyperlink ref="D15" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -4926,142 +4978,142 @@
   </cols>
   <sheetData>
     <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="68">
+      <c r="F11" s="67">
         <v>1</v>
       </c>
-      <c r="K11" s="69" t="s">
+      <c r="K11" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="69" t="s">
+      <c r="L11" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="70">
+      <c r="M11" s="69">
         <v>41929.583333333336</v>
       </c>
-      <c r="N11" s="71" t="s">
+      <c r="N11" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="71" t="s">
+      <c r="O11" s="70" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="72"/>
-      <c r="G12" s="73" t="s">
+      <c r="F12" s="71"/>
+      <c r="G12" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="74">
+      <c r="J12" s="73">
         <v>2</v>
       </c>
-      <c r="K12" s="75" t="s">
+      <c r="K12" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="75" t="s">
+      <c r="L12" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="76">
+      <c r="M12" s="75">
         <v>41933.475694444445</v>
       </c>
-      <c r="N12" s="77" t="s">
+      <c r="N12" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="77" t="s">
+      <c r="O12" s="76" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="78"/>
-      <c r="G13" s="79" t="s">
+      <c r="F13" s="77"/>
+      <c r="G13" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="79" t="s">
+      <c r="I13" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="J13" s="80">
+      <c r="J13" s="79">
         <v>3</v>
       </c>
-      <c r="K13" s="81" t="s">
+      <c r="K13" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="M13" s="82">
+      <c r="M13" s="81">
         <v>41939.449386574073</v>
       </c>
-      <c r="N13" s="71" t="s">
+      <c r="N13" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="O13" s="71" t="s">
+      <c r="O13" s="70" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="72"/>
-      <c r="G14" s="73" t="s">
+      <c r="F14" s="71"/>
+      <c r="G14" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="73" t="s">
+      <c r="I14" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="74">
+      <c r="J14" s="73">
         <v>4</v>
       </c>
-      <c r="K14" s="75" t="s">
+      <c r="K14" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="75" t="s">
+      <c r="L14" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="76">
+      <c r="M14" s="75">
         <v>41941.431875000002</v>
       </c>
-      <c r="N14" s="77" t="s">
+      <c r="N14" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="O14" s="77" t="s">
+      <c r="O14" s="76" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="78"/>
-      <c r="G15" s="79" t="s">
+      <c r="F15" s="77"/>
+      <c r="G15" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="I15" s="79" t="s">
+      <c r="I15" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="80">
+      <c r="J15" s="79">
         <v>5</v>
       </c>
-      <c r="K15" s="81" t="s">
+      <c r="K15" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="80" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="82">
+      <c r="M15" s="81">
         <v>41948.662094907406</v>
       </c>
-      <c r="N15" s="71" t="s">
+      <c r="N15" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="71" t="s">
+      <c r="O15" s="70" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved some bugs for iteration 7
Solved bug 2,3,7 and 8
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="158">
   <si>
     <t>S/N</t>
   </si>
@@ -488,13 +488,25 @@
   </si>
   <si>
     <t xml:space="preserve">Unable to click Route drop down list </t>
+  </si>
+  <si>
+    <t>Editted the sql query in frequencyDAO</t>
+  </si>
+  <si>
+    <t>Editted the sql query in routeDAO</t>
+  </si>
+  <si>
+    <t>Added new method in MedicationHistoryDAO and editted ProcessResetScenario</t>
+  </si>
+  <si>
+    <t>Checked for null scenario and added error message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +575,18 @@
       <sz val="10"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -768,7 +792,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -917,97 +941,94 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="10" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="9" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="10" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="10" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1064,28 +1085,43 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2109,28 +2145,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="87"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="89"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2139,30 +2175,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="87"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="86"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2598,28 +2634,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="87"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="89"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2628,30 +2664,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="87"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="86"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2948,28 +2984,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="87"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="89"/>
+      <c r="C4" s="88"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -2978,30 +3014,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="87"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="86"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3299,28 +3335,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="91"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="94"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3329,30 +3365,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="96"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="92"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="91"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3644,28 +3680,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="91"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="94"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3674,30 +3710,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="96"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="92"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="91"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4090,26 +4126,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="100"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="102"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4118,30 +4154,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="96"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="99"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4478,8 +4514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:L6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4502,26 +4538,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="100"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="102"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4530,33 +4566,33 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="96"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="99"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="81" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4565,16 +4601,16 @@
       <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="81" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="81" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -4583,24 +4619,24 @@
       <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="54" t="s">
+      <c r="K7" s="81" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="30">
         <v>1</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="103" t="s">
         <v>119</v>
       </c>
       <c r="F8" s="32">
@@ -4613,22 +4649,20 @@
         <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="31" t="s">
-        <v>124</v>
-      </c>
+      <c r="I8" s="31"/>
       <c r="J8" s="31"/>
       <c r="K8" s="35"/>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:17" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="46"/>
-      <c r="B9" s="28">
+      <c r="B9" s="104">
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="105" t="s">
         <v>118</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -4645,11 +4679,17 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+        <v>57</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="K9" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="36">
+        <v>42027</v>
+      </c>
       <c r="M9" s="46"/>
       <c r="N9" s="46"/>
       <c r="O9" s="46"/>
@@ -4658,16 +4698,16 @@
     </row>
     <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="46"/>
-      <c r="B10" s="28">
+      <c r="B10" s="104">
         <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="60" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="32">
@@ -4676,16 +4716,22 @@
       <c r="G10" s="30">
         <v>1</v>
       </c>
-      <c r="H10" s="56" t="str">
+      <c r="H10" s="54" t="str">
         <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I10" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
+      <c r="I10" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="36">
+        <v>42027</v>
+      </c>
       <c r="M10" s="46"/>
       <c r="N10" s="46"/>
       <c r="O10" s="46"/>
@@ -4697,10 +4743,10 @@
       <c r="B11" s="30">
         <v>4</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="107" t="s">
         <v>126</v>
       </c>
       <c r="E11" s="31" t="s">
@@ -4712,20 +4758,20 @@
       <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="64" t="str">
+      <c r="H11" s="62" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="66">
+      <c r="L11" s="64">
         <v>42026</v>
       </c>
       <c r="M11" s="46"/>
@@ -4734,15 +4780,15 @@
       <c r="P11" s="46"/>
       <c r="Q11" s="46"/>
     </row>
-    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="46"/>
-      <c r="B12" s="26">
+      <c r="B12" s="106">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="107" t="s">
         <v>126</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -4761,8 +4807,8 @@
       <c r="I12" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="61"/>
-      <c r="L12" s="60"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
@@ -4770,108 +4816,124 @@
       <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
-      <c r="B13" s="83">
+      <c r="A13" s="80"/>
+      <c r="B13" s="108">
         <v>6</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="108" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="61" t="s">
         <v>148</v>
       </c>
       <c r="F13" s="36">
         <v>42024</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="57">
         <v>5</v>
       </c>
-      <c r="H13" s="57" t="str">
+      <c r="H13" s="55" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
-    </row>
-    <row r="14" spans="1:17" s="103" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104"/>
-      <c r="B14" s="105">
+      <c r="J13" s="63"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+    </row>
+    <row r="14" spans="1:17" s="82" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="83"/>
+      <c r="B14" s="110">
         <v>7</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="108" t="s">
+      <c r="D14" s="111" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="F14" s="110">
+      <c r="F14" s="112">
         <v>42025</v>
       </c>
-      <c r="G14" s="105">
+      <c r="G14" s="110">
         <v>1</v>
       </c>
-      <c r="H14" s="57" t="str">
+      <c r="H14" s="55" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-    </row>
-    <row r="15" spans="1:17" s="103" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104"/>
-      <c r="B15" s="107">
+      <c r="I14" s="110" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="110" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="36">
+        <v>42027</v>
+      </c>
+      <c r="M14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+    </row>
+    <row r="15" spans="1:17" s="82" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="83"/>
+      <c r="B15" s="113">
         <v>8</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="109" t="s">
+      <c r="D15" s="114" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="107" t="s">
+      <c r="E15" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="110">
+      <c r="F15" s="112">
         <v>42025</v>
       </c>
-      <c r="G15" s="107">
+      <c r="G15" s="113">
         <v>1</v>
       </c>
-      <c r="H15" s="59" t="str">
+      <c r="H15" s="57" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I15" s="107"/>
-      <c r="J15" s="107"/>
-      <c r="K15" s="107"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
+      <c r="I15" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="K15" s="113" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="36">
+        <v>42027</v>
+      </c>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="46"/>
@@ -4978,142 +5040,142 @@
   </cols>
   <sheetData>
     <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="67">
+      <c r="F11" s="65">
         <v>1</v>
       </c>
-      <c r="K11" s="68" t="s">
+      <c r="K11" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="68" t="s">
+      <c r="L11" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="69">
+      <c r="M11" s="67">
         <v>41929.583333333336</v>
       </c>
-      <c r="N11" s="70" t="s">
+      <c r="N11" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="70" t="s">
+      <c r="O11" s="68" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="71"/>
-      <c r="G12" s="72" t="s">
+      <c r="F12" s="69"/>
+      <c r="G12" s="70" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="I12" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="71">
         <v>2</v>
       </c>
-      <c r="K12" s="74" t="s">
+      <c r="K12" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="75">
+      <c r="M12" s="73">
         <v>41933.475694444445</v>
       </c>
-      <c r="N12" s="76" t="s">
+      <c r="N12" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="76" t="s">
+      <c r="O12" s="74" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="77"/>
-      <c r="G13" s="78" t="s">
+      <c r="F13" s="75"/>
+      <c r="G13" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="J13" s="79">
+      <c r="J13" s="77">
         <v>3</v>
       </c>
-      <c r="K13" s="80" t="s">
+      <c r="K13" s="78" t="s">
         <v>139</v>
       </c>
-      <c r="L13" s="80" t="s">
+      <c r="L13" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="M13" s="81">
+      <c r="M13" s="79">
         <v>41939.449386574073</v>
       </c>
-      <c r="N13" s="70" t="s">
+      <c r="N13" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="O13" s="70" t="s">
+      <c r="O13" s="68" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="71"/>
-      <c r="G14" s="72" t="s">
+      <c r="F14" s="69"/>
+      <c r="G14" s="70" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="72" t="s">
+      <c r="H14" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="72" t="s">
+      <c r="I14" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="73">
+      <c r="J14" s="71">
         <v>4</v>
       </c>
-      <c r="K14" s="74" t="s">
+      <c r="K14" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="75">
+      <c r="M14" s="73">
         <v>41941.431875000002</v>
       </c>
-      <c r="N14" s="76" t="s">
+      <c r="N14" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="O14" s="76" t="s">
+      <c r="O14" s="74" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="77"/>
-      <c r="G15" s="78" t="s">
+      <c r="F15" s="75"/>
+      <c r="G15" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="I15" s="78" t="s">
+      <c r="I15" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="79">
+      <c r="J15" s="77">
         <v>5</v>
       </c>
-      <c r="K15" s="80" t="s">
+      <c r="K15" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="80" t="s">
+      <c r="L15" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="81">
+      <c r="M15" s="79">
         <v>41948.662094907406</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="N15" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="70" t="s">
+      <c r="O15" s="68" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Debugged remaining bugs for iteration 7
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="161">
   <si>
     <t>S/N</t>
   </si>
@@ -496,10 +496,19 @@
     <t>Editted the sql query in routeDAO</t>
   </si>
   <si>
-    <t>Added new method in MedicationHistoryDAO and editted ProcessResetScenario</t>
-  </si>
-  <si>
     <t>Checked for null scenario and added error message</t>
+  </si>
+  <si>
+    <t>Can't find error</t>
+  </si>
+  <si>
+    <t>Added new method in MedicationHistoryDAO and edited ProcessResetScenario</t>
+  </si>
+  <si>
+    <t>Changed the sql statement in VitalDAO</t>
+  </si>
+  <si>
+    <t>Set default gender as Male to avoid this error</t>
   </si>
 </sst>
 </file>
@@ -590,7 +599,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +633,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDFDFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,7 +807,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -953,12 +968,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -968,9 +977,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1031,6 +1037,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1085,43 +1130,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2145,28 +2154,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="88"/>
+      <c r="C4" s="98"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2175,30 +2184,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="86"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2634,28 +2643,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="88"/>
+      <c r="C4" s="98"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2664,30 +2673,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="86"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2984,28 +2993,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="88"/>
+      <c r="C4" s="98"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -3014,30 +3023,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="86"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3335,28 +3344,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="91"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="101"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3365,30 +3374,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="91"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3680,28 +3689,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="91"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="101"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3710,30 +3719,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="91"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4126,26 +4135,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="109"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="101"/>
+      <c r="C4" s="111"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4154,30 +4163,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="109"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4514,8 +4523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4538,26 +4547,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="109"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="101"/>
+      <c r="C4" s="111"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4566,33 +4575,33 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="109"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="78" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4601,16 +4610,16 @@
       <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="78" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="81" t="s">
+      <c r="G7" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="81" t="s">
+      <c r="H7" s="78" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -4619,7 +4628,7 @@
       <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="81" t="s">
+      <c r="K7" s="78" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -4633,10 +4642,10 @@
       <c r="C8" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="103" t="s">
+      <c r="E8" s="82" t="s">
         <v>119</v>
       </c>
       <c r="F8" s="32">
@@ -4649,20 +4658,28 @@
         <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
+      <c r="I8" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="36">
+        <v>42028</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="46"/>
-      <c r="B9" s="104">
+      <c r="B9" s="83">
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="84" t="s">
         <v>118</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -4682,9 +4699,9 @@
         <v>57</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="K9" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="K9" s="61" t="s">
         <v>68</v>
       </c>
       <c r="L9" s="36">
@@ -4698,16 +4715,16 @@
     </row>
     <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="46"/>
-      <c r="B10" s="104">
+      <c r="B10" s="83">
         <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="102" t="s">
+      <c r="D10" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="58" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="32">
@@ -4724,7 +4741,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>68</v>
@@ -4743,10 +4760,10 @@
       <c r="B11" s="30">
         <v>4</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="107" t="s">
+      <c r="D11" s="86" t="s">
         <v>126</v>
       </c>
       <c r="E11" s="31" t="s">
@@ -4758,20 +4775,20 @@
       <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="62" t="str">
+      <c r="H11" s="60" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="64">
+      <c r="L11" s="61">
         <v>42026</v>
       </c>
       <c r="M11" s="46"/>
@@ -4782,13 +4799,13 @@
     </row>
     <row r="12" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="46"/>
-      <c r="B12" s="106">
+      <c r="B12" s="85">
         <v>5</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="107" t="s">
+      <c r="D12" s="86" t="s">
         <v>126</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -4805,10 +4822,17 @@
         <v>Low Impact</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="K12" s="59"/>
-      <c r="L12" s="58"/>
+        <v>57</v>
+      </c>
+      <c r="J12" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="K12" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="36">
+        <v>42028</v>
+      </c>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
@@ -4816,17 +4840,17 @@
       <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="80"/>
-      <c r="B13" s="108">
+      <c r="A13" s="77"/>
+      <c r="B13" s="87">
         <v>6</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="87" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="59" t="s">
         <v>148</v>
       </c>
       <c r="F13" s="36">
@@ -4842,98 +4866,102 @@
       <c r="I13" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="112" t="s">
+        <v>157</v>
+      </c>
+      <c r="K13" s="59" t="s">
+        <v>55</v>
+      </c>
       <c r="L13" s="56"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="80"/>
-    </row>
-    <row r="14" spans="1:17" s="82" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="110">
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77"/>
+      <c r="Q13" s="77"/>
+    </row>
+    <row r="14" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="80"/>
+      <c r="B14" s="89">
         <v>7</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="111" t="s">
+      <c r="D14" s="90" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="110" t="s">
+      <c r="E14" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="F14" s="112">
+      <c r="F14" s="91">
         <v>42025</v>
       </c>
-      <c r="G14" s="110">
+      <c r="G14" s="89">
         <v>1</v>
       </c>
       <c r="H14" s="55" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I14" s="110" t="s">
+      <c r="I14" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="110" t="s">
+      <c r="J14" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="K14" s="110" t="s">
+      <c r="K14" s="89" t="s">
         <v>68</v>
       </c>
       <c r="L14" s="36">
         <v>42027</v>
       </c>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
-    </row>
-    <row r="15" spans="1:17" s="82" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="113">
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+    </row>
+    <row r="15" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="80"/>
+      <c r="B15" s="92">
         <v>8</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="114" t="s">
+      <c r="D15" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="113" t="s">
+      <c r="E15" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="112">
+      <c r="F15" s="91">
         <v>42025</v>
       </c>
-      <c r="G15" s="113">
+      <c r="G15" s="92">
         <v>1</v>
       </c>
       <c r="H15" s="57" t="str">
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I15" s="113" t="s">
+      <c r="I15" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="113" t="s">
+      <c r="J15" s="92" t="s">
         <v>155</v>
       </c>
-      <c r="K15" s="113" t="s">
+      <c r="K15" s="92" t="s">
         <v>68</v>
       </c>
       <c r="L15" s="36">
         <v>42027</v>
       </c>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="46"/>
@@ -5040,142 +5068,142 @@
   </cols>
   <sheetData>
     <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="65">
+      <c r="F11" s="62">
         <v>1</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="66" t="s">
+      <c r="L11" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="67">
+      <c r="M11" s="64">
         <v>41929.583333333336</v>
       </c>
-      <c r="N11" s="68" t="s">
+      <c r="N11" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="68" t="s">
+      <c r="O11" s="65" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="69"/>
-      <c r="G12" s="70" t="s">
+      <c r="F12" s="66"/>
+      <c r="G12" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="71">
+      <c r="J12" s="68">
         <v>2</v>
       </c>
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="72" t="s">
+      <c r="L12" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="73">
+      <c r="M12" s="70">
         <v>41933.475694444445</v>
       </c>
-      <c r="N12" s="74" t="s">
+      <c r="N12" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="74" t="s">
+      <c r="O12" s="71" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="75"/>
-      <c r="G13" s="76" t="s">
+      <c r="F13" s="72"/>
+      <c r="G13" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="76" t="s">
+      <c r="I13" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="J13" s="77">
+      <c r="J13" s="74">
         <v>3</v>
       </c>
-      <c r="K13" s="78" t="s">
+      <c r="K13" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="L13" s="78" t="s">
+      <c r="L13" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="M13" s="79">
+      <c r="M13" s="76">
         <v>41939.449386574073</v>
       </c>
-      <c r="N13" s="68" t="s">
+      <c r="N13" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="O13" s="68" t="s">
+      <c r="O13" s="65" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="69"/>
-      <c r="G14" s="70" t="s">
+      <c r="F14" s="66"/>
+      <c r="G14" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="70" t="s">
+      <c r="H14" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="70" t="s">
+      <c r="I14" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="71">
+      <c r="J14" s="68">
         <v>4</v>
       </c>
-      <c r="K14" s="72" t="s">
+      <c r="K14" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="73">
+      <c r="M14" s="70">
         <v>41941.431875000002</v>
       </c>
-      <c r="N14" s="74" t="s">
+      <c r="N14" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="O14" s="74" t="s">
+      <c r="O14" s="71" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="75"/>
-      <c r="G15" s="76" t="s">
+      <c r="F15" s="72"/>
+      <c r="G15" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="76" t="s">
+      <c r="H15" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="I15" s="76" t="s">
+      <c r="I15" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="77">
+      <c r="J15" s="74">
         <v>5</v>
       </c>
-      <c r="K15" s="78" t="s">
+      <c r="K15" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="78" t="s">
+      <c r="L15" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="79">
+      <c r="M15" s="76">
         <v>41948.662094907406</v>
       </c>
-      <c r="N15" s="68" t="s">
+      <c r="N15" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="O15" s="68" t="s">
+      <c r="O15" s="65" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All test cases for iteration 7 passed
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="157">
   <si>
     <t>S/N</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Error message should be displayed when no case is activated</t>
   </si>
   <si>
-    <t>unsolved</t>
-  </si>
-  <si>
     <t>Case Setup - State V2</t>
   </si>
   <si>
@@ -469,12 +466,6 @@
     <t>SC4</t>
   </si>
   <si>
-    <t>Activate Case</t>
-  </si>
-  <si>
-    <t>Null pointer in student portal when admin activate case</t>
-  </si>
-  <si>
     <t>Added required for case name</t>
   </si>
   <si>
@@ -497,9 +488,6 @@
   </si>
   <si>
     <t>Checked for null scenario and added error message</t>
-  </si>
-  <si>
-    <t>Can't find error</t>
   </si>
   <si>
     <t>Added new method in MedicationHistoryDAO and edited ProcessResetScenario</t>
@@ -515,7 +503,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,8 +586,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,12 +626,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDFDFDF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,18 +949,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,9 +1036,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1070,12 +1045,6 @@
     <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1130,8 +1099,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2154,28 +2141,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="90"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2184,30 +2171,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2643,28 +2630,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="90"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2673,30 +2660,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2993,28 +2980,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="90"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -3023,30 +3010,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3344,28 +3331,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="95"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3374,30 +3361,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="95"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3689,28 +3676,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="95"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3719,30 +3706,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="95"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4135,26 +4122,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="111"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4163,30 +4150,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="103"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4523,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4547,61 +4534,61 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="111"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="103"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="75" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4610,16 +4597,16 @@
       <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="78" t="s">
+      <c r="E7" s="75" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="75" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -4628,7 +4615,7 @@
       <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="78" t="s">
+      <c r="K7" s="75" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -4642,10 +4629,10 @@
       <c r="C8" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="79" t="s">
         <v>119</v>
       </c>
       <c r="F8" s="32">
@@ -4658,28 +4645,28 @@
         <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="K8" s="35" t="s">
+      <c r="J8" s="106" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8" s="108">
         <v>42028</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="46"/>
-      <c r="B9" s="83">
+      <c r="B9" s="80">
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="81" t="s">
         <v>118</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -4699,9 +4686,9 @@
         <v>57</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="K9" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="58" t="s">
         <v>68</v>
       </c>
       <c r="L9" s="36">
@@ -4715,16 +4702,16 @@
     </row>
     <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="46"/>
-      <c r="B10" s="83">
+      <c r="B10" s="80">
         <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="56" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="32">
@@ -4741,7 +4728,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>68</v>
@@ -4760,14 +4747,14 @@
       <c r="B11" s="30">
         <v>4</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="82" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="E11" s="31" t="s">
         <v>126</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>127</v>
       </c>
       <c r="F11" s="36">
         <v>42024</v>
@@ -4775,20 +4762,20 @@
       <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="60" t="str">
+      <c r="H11" s="57" t="str">
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="K11" s="61" t="s">
+      <c r="J11" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="K11" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="61">
+      <c r="L11" s="58">
         <v>42026</v>
       </c>
       <c r="M11" s="46"/>
@@ -4799,17 +4786,17 @@
     </row>
     <row r="12" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="46"/>
-      <c r="B12" s="85">
+      <c r="B12" s="82">
         <v>5</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="82" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="86" t="s">
-        <v>126</v>
-      </c>
       <c r="E12" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="36">
         <v>42024</v>
@@ -4824,10 +4811,10 @@
       <c r="I12" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="79" t="s">
-        <v>160</v>
-      </c>
-      <c r="K12" s="89" t="s">
+      <c r="J12" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="K12" s="85" t="s">
         <v>55</v>
       </c>
       <c r="L12" s="36">
@@ -4839,145 +4826,124 @@
       <c r="P12" s="46"/>
       <c r="Q12" s="46"/>
     </row>
-    <row r="13" spans="1:17" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="77"/>
-      <c r="B13" s="87">
+    <row r="13" spans="1:17" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="74"/>
+      <c r="B13" s="84">
         <v>6</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="88" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="59" t="s">
+      <c r="D13" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="F13" s="36">
-        <v>42024</v>
-      </c>
-      <c r="G13" s="57">
-        <v>5</v>
+      <c r="E13" s="85" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="87">
+        <v>42025</v>
+      </c>
+      <c r="G13" s="85">
+        <v>1</v>
       </c>
       <c r="H13" s="55" t="str">
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v xml:space="preserve">High Impact </v>
-      </c>
-      <c r="I13" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="J13" s="112" t="s">
-        <v>157</v>
-      </c>
-      <c r="K13" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" s="56"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="77"/>
-    </row>
-    <row r="14" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
-      <c r="B14" s="89">
+        <v>Low Impact</v>
+      </c>
+      <c r="I13" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="85" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="36">
+        <v>42027</v>
+      </c>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+    </row>
+    <row r="14" spans="1:17" s="76" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="77"/>
+      <c r="B14" s="85">
         <v>7</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="90" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" s="91">
+      <c r="F14" s="87">
         <v>42025</v>
       </c>
-      <c r="G14" s="89">
+      <c r="G14" s="85">
         <v>1</v>
       </c>
-      <c r="H14" s="55" t="str">
+      <c r="H14" s="31" t="str">
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="89" t="s">
-        <v>154</v>
-      </c>
-      <c r="K14" s="89" t="s">
+      <c r="J14" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="85" t="s">
         <v>68</v>
       </c>
       <c r="L14" s="36">
         <v>42027</v>
       </c>
-      <c r="M14" s="80"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="80"/>
-    </row>
-    <row r="15" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
-      <c r="B15" s="92">
-        <v>8</v>
-      </c>
-      <c r="C15" s="89" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="93" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="92" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="91">
-        <v>42025</v>
-      </c>
-      <c r="G15" s="92">
-        <v>1</v>
-      </c>
-      <c r="H15" s="57" t="str">
-        <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v>Low Impact</v>
-      </c>
-      <c r="I15" s="92" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="92" t="s">
-        <v>155</v>
-      </c>
-      <c r="K15" s="92" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="36">
-        <v>42027</v>
-      </c>
-      <c r="M15" s="80"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="80"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="77"/>
+    </row>
+    <row r="15" spans="1:17" s="76" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="77"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
       <c r="H16" s="51" t="str">
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="46"/>
@@ -5038,10 +5004,9 @@
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1"/>
     <hyperlink ref="D14" r:id="rId2"/>
-    <hyperlink ref="D15" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5068,143 +5033,143 @@
   </cols>
   <sheetData>
     <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="62">
+      <c r="F11" s="59">
         <v>1</v>
       </c>
-      <c r="K11" s="63" t="s">
+      <c r="K11" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="L11" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="63" t="s">
+      <c r="M11" s="61">
+        <v>41929.583333333336</v>
+      </c>
+      <c r="N11" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="64">
-        <v>41929.583333333336</v>
-      </c>
-      <c r="N11" s="65" t="s">
+      <c r="O11" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="65" t="s">
+    </row>
+    <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="63"/>
+      <c r="G12" s="64" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="66"/>
-      <c r="G12" s="67" t="s">
+      <c r="H12" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="67" t="s">
+      <c r="I12" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="67" t="s">
+      <c r="J12" s="65">
+        <v>2</v>
+      </c>
+      <c r="K12" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="J12" s="68">
-        <v>2</v>
-      </c>
-      <c r="K12" s="69" t="s">
+      <c r="L12" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="69" t="s">
+      <c r="M12" s="67">
+        <v>41933.475694444445</v>
+      </c>
+      <c r="N12" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="70">
-        <v>41933.475694444445</v>
-      </c>
-      <c r="N12" s="71" t="s">
+      <c r="O12" s="68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="69"/>
+      <c r="G13" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="71">
+        <v>3</v>
+      </c>
+      <c r="K13" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="71" t="s">
+      <c r="L13" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="M13" s="73">
+        <v>41939.449386574073</v>
+      </c>
+      <c r="N13" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="O13" s="62" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="F14" s="63"/>
+      <c r="G14" s="64" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="72"/>
-      <c r="G13" s="73" t="s">
+      <c r="H14" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="I14" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" s="74">
-        <v>3</v>
-      </c>
-      <c r="K13" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="L13" s="75" t="s">
+      <c r="J14" s="65">
+        <v>4</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="M14" s="67">
+        <v>41941.431875000002</v>
+      </c>
+      <c r="N14" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="M13" s="76">
-        <v>41939.449386574073</v>
-      </c>
-      <c r="N13" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="O13" s="65" t="s">
+      <c r="O14" s="68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F15" s="69"/>
+      <c r="G15" s="70" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="66"/>
-      <c r="G14" s="67" t="s">
+      <c r="H15" s="70" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="67" t="s">
+      <c r="I15" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="J14" s="68">
-        <v>4</v>
-      </c>
-      <c r="K14" s="69" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14" s="69" t="s">
+      <c r="J15" s="71">
+        <v>5</v>
+      </c>
+      <c r="K15" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="M14" s="70">
-        <v>41941.431875000002</v>
-      </c>
-      <c r="N14" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="O14" s="71" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="72"/>
-      <c r="G15" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J15" s="74">
-        <v>5</v>
-      </c>
-      <c r="K15" s="75" t="s">
+      <c r="L15" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="75" t="s">
+      <c r="M15" s="73">
+        <v>41948.662094907406</v>
+      </c>
+      <c r="N15" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="O15" s="62" t="s">
         <v>145</v>
-      </c>
-      <c r="M15" s="76">
-        <v>41948.662094907406</v>
-      </c>
-      <c r="N15" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="O15" s="65" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated metrics for iteration 7
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="5" activeTab="6"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -1076,6 +1076,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,9 +1132,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2154,28 +2154,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="99"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -2184,30 +2184,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="97"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -2643,28 +2643,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="99"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -2673,30 +2673,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="97"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -2993,28 +2993,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="99"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -3023,30 +3023,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="97"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -3344,28 +3344,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -3374,30 +3374,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="102"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -3689,28 +3689,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -3719,30 +3719,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="102"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -4135,26 +4135,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="111"/>
+      <c r="C4" s="112"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4163,30 +4163,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -4523,8 +4523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4547,26 +4547,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="111"/>
+      <c r="C4" s="112"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -4575,30 +4575,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="78" t="s">
@@ -4866,7 +4866,7 @@
       <c r="I13" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="112" t="s">
+      <c r="J13" s="94" t="s">
         <v>157</v>
       </c>
       <c r="K13" s="59" t="s">
@@ -5050,7 +5050,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="F11:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Redraw Bug Score and Metric Chart
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Iteration 7" sheetId="10" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="11" r:id="rId8"/>
     <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId9"/>
+    <sheet name="Overview" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="164">
   <si>
     <t>S/N</t>
   </si>
@@ -509,13 +510,22 @@
   </si>
   <si>
     <t>Set default gender as Male to avoid this error</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +608,14 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -643,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -801,13 +819,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1133,6 +1166,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1150,6 +1186,2787 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Critical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{D081A671-221C-445B-8A2B-BBED0E2AC233}" type="VALUE">
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr>
+                        <a:defRPr sz="1100"/>
+                      </a:pPr>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-SG"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="346504512"/>
+        <c:axId val="346515392"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="122D4E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="picture"/>
+            <c:spPr>
+              <a:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.0100250626566414E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.6783625730994274E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.6783625730994212E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3567944803858045E-2"/>
+                  <c:y val="-6.6833751044277356E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8002572281046428E-2"/>
+                  <c:y val="-4.0100250626566449E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6422463092490819E-2"/>
+                  <c:y val="-2.6733500417711005E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.8298246964468768E-3"/>
+                  <c:y val="-2.6733500417710943E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="346504512"/>
+        <c:axId val="346515392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="346504512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG" sz="1800"/>
+                  <a:t>Iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346515392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346515392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346504512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Critical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{D081A671-221C-445B-8A2B-BBED0E2AC233}" type="VALUE">
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr>
+                        <a:defRPr sz="1100"/>
+                      </a:pPr>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-SG"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="346275296"/>
+        <c:axId val="346276928"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="122D4E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="picture"/>
+            <c:spPr>
+              <a:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </a:blipFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.0100250626566414E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.6783625730994274E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5844561362190865E-2"/>
+                  <c:y val="-4.6783625730994212E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3567944803858045E-2"/>
+                  <c:y val="-6.6833751044277356E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8002572281046428E-2"/>
+                  <c:y val="-4.0100250626566449E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6422463092490819E-2"/>
+                  <c:y val="-2.6733500417711005E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.8298246964468768E-3"/>
+                  <c:y val="-2.6733500417710943E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Overview!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="346275296"/>
+        <c:axId val="346276928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="346275296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG" sz="1800"/>
+                  <a:t>Iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346276928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346276928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346275296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1841,6 +4658,75 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>325531</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>358587</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>373235</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2615,6 +5501,155 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" s="114" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="115" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="115" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="115" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="115" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="113">
+        <v>1</v>
+      </c>
+      <c r="C3" s="113">
+        <v>9</v>
+      </c>
+      <c r="D3" s="113">
+        <v>1</v>
+      </c>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113">
+        <f>(C3*1)+(D3*5)+(E3*10)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="113">
+        <v>2</v>
+      </c>
+      <c r="C4" s="113">
+        <v>1</v>
+      </c>
+      <c r="D4" s="113">
+        <v>2</v>
+      </c>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113">
+        <f>(C4*1)+(D4*5)+(E4*10)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="113">
+        <v>3</v>
+      </c>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113">
+        <v>3</v>
+      </c>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113">
+        <f>(C5*1)+(D5*5)+(E5*10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="113">
+        <v>4</v>
+      </c>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113">
+        <v>1</v>
+      </c>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113">
+        <f>(C6*1)+(D6*5)+(E6*10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="113">
+        <v>5</v>
+      </c>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113">
+        <v>6</v>
+      </c>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113">
+        <f>(C7*1)+(D7*5)+(E7*10)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="113">
+        <v>6</v>
+      </c>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113">
+        <v>4</v>
+      </c>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113">
+        <f>(C8*1)+(D8*5)+(E8*10)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="113">
+        <v>7</v>
+      </c>
+      <c r="C9" s="113">
+        <v>5</v>
+      </c>
+      <c r="D9" s="113">
+        <v>3</v>
+      </c>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113">
+        <f>(C9*1)+(D9*5)+(E9*10)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="113"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
@@ -4523,7 +7558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -5050,7 +8085,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="F11:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
solved some bugs for iteration 8
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="201">
   <si>
     <t>S/N</t>
   </si>
@@ -601,13 +601,43 @@
   </si>
   <si>
     <t>Information displayed is wrong for multidisciplinary notes tab</t>
+  </si>
+  <si>
+    <t>Corrected validation and allowed numbers</t>
+  </si>
+  <si>
+    <t>Solved Partially</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weiyi, can you add error and success message for this? Thanks! I set it in ProcessRetrieveNotesByPracticalGroup alr, but can't show in viewSubmissionLecturer.jsp </t>
+  </si>
+  <si>
+    <t>Added two dropdown (Scenario Name and practical group) , for lecturer to view .</t>
+  </si>
+  <si>
+    <t>Path changed to openshift's path in ProcessReportUpload</t>
+  </si>
+  <si>
+    <t>Path changed to openshift's path in ProcessDocumentUpload</t>
+  </si>
+  <si>
+    <t>Added a hidden attribute to determine which page the user is coming from</t>
+  </si>
+  <si>
+    <t>Is this due to the upload link? Don't uds the error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this due to the upload link? Don't uds the error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed "Medication" to Multidisciplinary" </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,6 +734,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -940,7 +989,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1218,6 +1267,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1272,44 +1360,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1417,7 +1475,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1519,7 +1576,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1637,7 +1693,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SG"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1740,8 +1796,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="241401352"/>
-        <c:axId val="186087840"/>
+        <c:axId val="1649693568"/>
+        <c:axId val="1649685952"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1801,9 +1857,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1822,9 +1876,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1843,9 +1895,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1864,9 +1914,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1885,9 +1933,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1906,9 +1952,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1927,9 +1971,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2031,11 +2073,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="241401352"/>
-        <c:axId val="186087840"/>
+        <c:axId val="1649693568"/>
+        <c:axId val="1649685952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241401352"/>
+        <c:axId val="1649693568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,7 +2109,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2114,7 +2155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186087840"/>
+        <c:crossAx val="1649685952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2122,7 +2163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186087840"/>
+        <c:axId val="1649685952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241401352"/>
+        <c:crossAx val="1649693568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2173,7 +2214,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2329,7 +2369,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-SG"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2432,8 +2472,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="247686568"/>
-        <c:axId val="247686960"/>
+        <c:axId val="1922915536"/>
+        <c:axId val="1922914992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2493,9 +2533,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2514,9 +2552,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2535,9 +2571,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2556,9 +2590,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2577,9 +2609,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2598,9 +2628,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2619,9 +2647,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2723,11 +2749,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="247686568"/>
-        <c:axId val="247686960"/>
+        <c:axId val="1922915536"/>
+        <c:axId val="1922914992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247686568"/>
+        <c:axId val="1922915536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2759,7 +2785,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2806,7 +2831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247686960"/>
+        <c:crossAx val="1922914992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2814,7 +2839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247686960"/>
+        <c:axId val="1922914992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,7 +2876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247686568"/>
+        <c:crossAx val="1922915536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2865,7 +2890,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4003,28 +4027,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="114"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="116"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -4033,30 +4057,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="G4" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -4789,28 +4813,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="114"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="116"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -4819,30 +4843,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="G4" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -5139,28 +5163,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="114"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="116"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -5169,30 +5193,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="G4" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -5490,28 +5514,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="106"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="119"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="108"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -5520,30 +5544,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -5835,28 +5859,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="106"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="119"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="108"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -5865,30 +5889,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -6281,26 +6305,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6309,30 +6333,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -6693,26 +6717,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6721,30 +6745,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="78" t="s">
@@ -7195,8 +7219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7219,26 +7243,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>56</v>
@@ -7247,30 +7271,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="95" t="s">
@@ -7311,10 +7335,10 @@
       <c r="B8" s="30">
         <v>1</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="102" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="121" t="s">
+      <c r="D8" s="103" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="82" t="s">
@@ -7330,20 +7354,28 @@
         <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="119"/>
+      <c r="I8" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="36">
+        <v>42043</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="79" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="101"/>
       <c r="B9" s="30">
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="100" t="s">
         <v>168</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -7359,25 +7391,35 @@
         <f>IFERROR(VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119"/>
-      <c r="Q9" s="119"/>
+      <c r="I9" s="131" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M9" s="130" t="s">
+        <v>193</v>
+      </c>
+      <c r="N9" s="101"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
     </row>
     <row r="10" spans="1:17" s="79" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="119"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="30">
         <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="103" t="s">
         <v>172</v>
       </c>
       <c r="E10" s="58" t="s">
@@ -7393,25 +7435,33 @@
         <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="119"/>
-      <c r="Q10" s="119"/>
+      <c r="I10" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
     </row>
     <row r="11" spans="1:17" s="79" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="119"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="30">
         <v>4</v>
       </c>
       <c r="C11" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="104" t="s">
         <v>172</v>
       </c>
       <c r="E11" s="58" t="s">
@@ -7427,25 +7477,33 @@
         <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="119"/>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
+      <c r="I11" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M11" s="101"/>
+      <c r="N11" s="101"/>
+      <c r="O11" s="101"/>
+      <c r="P11" s="101"/>
+      <c r="Q11" s="101"/>
     </row>
     <row r="12" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="119"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="30">
         <v>5</v>
       </c>
       <c r="C12" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="104" t="s">
         <v>168</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -7464,11 +7522,11 @@
       <c r="I12" s="31"/>
       <c r="K12" s="89"/>
       <c r="L12" s="36"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
-      <c r="Q12" s="119"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
     </row>
     <row r="13" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80"/>
@@ -7495,7 +7553,7 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I13" s="57"/>
-      <c r="J13" s="117"/>
+      <c r="J13" s="99"/>
       <c r="K13" s="59"/>
       <c r="L13" s="56"/>
       <c r="M13" s="80"/>
@@ -7512,7 +7570,7 @@
       <c r="C14" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="104" t="s">
         <v>180</v>
       </c>
       <c r="E14" s="89" t="s">
@@ -7562,27 +7620,35 @@
         <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="36"/>
+      <c r="I15" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="92" t="s">
+        <v>197</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="36">
+        <v>42043</v>
+      </c>
       <c r="M15" s="80"/>
       <c r="N15" s="80"/>
       <c r="O15" s="80"/>
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
     </row>
-    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="83.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="30">
         <v>9</v>
       </c>
-      <c r="C16" s="124" t="s">
+      <c r="C16" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="D16" s="126" t="s">
+      <c r="D16" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="E16" s="124" t="s">
+      <c r="E16" s="106" t="s">
         <v>186</v>
       </c>
       <c r="F16" s="32">
@@ -7596,21 +7662,24 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I16" s="92"/>
-      <c r="J16" s="127"/>
-      <c r="K16" s="124"/>
-      <c r="L16" s="128"/>
-    </row>
-    <row r="17" spans="2:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="123">
+      <c r="J16" s="109"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="132" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="105">
         <v>10</v>
       </c>
-      <c r="C17" s="125" t="s">
+      <c r="C17" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="D17" s="122" t="s">
+      <c r="D17" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="124" t="s">
+      <c r="E17" s="106" t="s">
         <v>187</v>
       </c>
       <c r="F17" s="32">
@@ -7624,21 +7693,24 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I17" s="92"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="124"/>
-      <c r="L17" s="128"/>
-    </row>
-    <row r="18" spans="2:12" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="123">
+      <c r="J17" s="109"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="132" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="105">
         <v>11</v>
       </c>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="D18" s="122" t="s">
+      <c r="D18" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="E18" s="129" t="s">
+      <c r="E18" s="111" t="s">
         <v>188</v>
       </c>
       <c r="F18" s="32">
@@ -7652,19 +7724,22 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I18" s="92"/>
-      <c r="J18" s="127"/>
-      <c r="K18" s="124"/>
-      <c r="L18" s="128"/>
-    </row>
-    <row r="19" spans="2:12" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="123">
+      <c r="J18" s="109"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="132" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="105">
         <v>12</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="122"/>
-      <c r="E19" s="129" t="s">
+      <c r="D19" s="104"/>
+      <c r="E19" s="111" t="s">
         <v>190</v>
       </c>
       <c r="F19" s="32">
@@ -7677,30 +7752,38 @@
         <f>IFERROR(VLOOKUP(G19,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I19" s="92"/>
-      <c r="J19" s="127"/>
-      <c r="K19" s="124"/>
-      <c r="L19" s="128"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I19" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="109" t="s">
+        <v>200</v>
+      </c>
+      <c r="K19" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="36">
+        <v>42043</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H20" s="51" t="str">
         <f>IFERROR(VLOOKUP(G20,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H21" s="51" t="str">
         <f>IFERROR(VLOOKUP(G21,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H22" s="49"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H23" s="49"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H24" s="49"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved all remaining bugs and modified Edit case
Shifted all creation to reveal modal (editState, editMedication)
Allow modification of doctor's order in edit state page and
update/insert to database
Changed report name to match database values
Display tables only when there are rows to show
Added linkedhashmap to statehistory to fix ordering of doctor order on
student portal
Add display of messages for viewSubmissionLecturer
Solved reset case bugs
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="201">
   <si>
     <t>S/N</t>
   </si>
@@ -606,12 +606,6 @@
     <t>Corrected validation and allowed numbers</t>
   </si>
   <si>
-    <t>Solved Partially</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weiyi, can you add error and success message for this? Thanks! I set it in ProcessRetrieveNotesByPracticalGroup alr, but can't show in viewSubmissionLecturer.jsp </t>
-  </si>
-  <si>
     <t>Added two dropdown (Scenario Name and practical group) , for lecturer to view .</t>
   </si>
   <si>
@@ -624,13 +618,19 @@
     <t>Added a hidden attribute to determine which page the user is coming from</t>
   </si>
   <si>
-    <t>Is this due to the upload link? Don't uds the error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is this due to the upload link? Don't uds the error. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Changed "Medication" to Multidisciplinary" </t>
+  </si>
+  <si>
+    <t>Format text to center</t>
+  </si>
+  <si>
+    <t>Modify SQL statement from Delete to Update</t>
+  </si>
+  <si>
+    <t>Remove reset statement</t>
+  </si>
+  <si>
+    <t>Redirected to Admin Homepage</t>
   </si>
 </sst>
 </file>
@@ -743,14 +743,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -989,7 +988,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1300,12 +1299,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,14 +1362,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1796,8 +1792,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1649693568"/>
-        <c:axId val="1649685952"/>
+        <c:axId val="190492000"/>
+        <c:axId val="190492392"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2073,11 +2069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1649693568"/>
-        <c:axId val="1649685952"/>
+        <c:axId val="190492000"/>
+        <c:axId val="190492392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1649693568"/>
+        <c:axId val="190492000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,7 +2151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649685952"/>
+        <c:crossAx val="190492392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2163,7 +2159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1649685952"/>
+        <c:axId val="190492392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2196,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1649693568"/>
+        <c:crossAx val="190492000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2472,8 +2468,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1922915536"/>
-        <c:axId val="1922914992"/>
+        <c:axId val="190493176"/>
+        <c:axId val="190493568"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2749,11 +2745,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1922915536"/>
-        <c:axId val="1922914992"/>
+        <c:axId val="190493176"/>
+        <c:axId val="190493568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1922915536"/>
+        <c:axId val="190493176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +2827,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1922914992"/>
+        <c:crossAx val="190493568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2839,7 +2835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1922914992"/>
+        <c:axId val="190493568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,7 +2872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1922915536"/>
+        <c:crossAx val="190493176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4027,28 +4023,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -4057,30 +4053,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="115" t="s">
+      <c r="G4" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -4813,28 +4809,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -4843,30 +4839,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="115" t="s">
+      <c r="G4" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -5163,28 +5159,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="115"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -5193,30 +5189,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="115" t="s">
+      <c r="G4" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -5514,28 +5510,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="120"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="121"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -5544,30 +5540,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="120"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -5859,28 +5855,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="120"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="121"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -5889,30 +5885,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="120"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -6305,26 +6301,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="129"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6333,30 +6329,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -6717,26 +6713,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="129"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6745,30 +6741,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="78" t="s">
@@ -7219,8 +7215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7243,26 +7239,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="126" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="129"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>56</v>
@@ -7271,30 +7267,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="95" t="s">
@@ -7367,7 +7363,7 @@
         <v>42043</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="79" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="101"/>
       <c r="B9" s="30">
         <v>2</v>
@@ -7392,10 +7388,10 @@
         <v xml:space="preserve">High Impact </v>
       </c>
       <c r="I9" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>192</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>194</v>
       </c>
       <c r="K9" s="61" t="s">
         <v>68</v>
@@ -7403,9 +7399,7 @@
       <c r="L9" s="36">
         <v>42043</v>
       </c>
-      <c r="M9" s="130" t="s">
-        <v>193</v>
-      </c>
+      <c r="M9" s="111"/>
       <c r="N9" s="101"/>
       <c r="O9" s="101"/>
       <c r="P9" s="101"/>
@@ -7439,7 +7433,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K10" s="36" t="s">
         <v>68</v>
@@ -7481,7 +7475,7 @@
         <v>57</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K11" s="36" t="s">
         <v>68</v>
@@ -7519,9 +7513,18 @@
         <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v>Low Impact</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="36"/>
+      <c r="I12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="K12" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="36">
+        <v>42043</v>
+      </c>
       <c r="M12" s="101"/>
       <c r="N12" s="101"/>
       <c r="O12" s="101"/>
@@ -7552,10 +7555,18 @@
         <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I13" s="57"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="56"/>
+      <c r="I13" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" s="56">
+        <v>42043</v>
+      </c>
       <c r="M13" s="80"/>
       <c r="N13" s="80"/>
       <c r="O13" s="80"/>
@@ -7586,10 +7597,18 @@
         <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="36"/>
+      <c r="I14" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="K14" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="36">
+        <v>42043</v>
+      </c>
       <c r="M14" s="80"/>
       <c r="N14" s="80"/>
       <c r="O14" s="80"/>
@@ -7624,7 +7643,7 @@
         <v>57</v>
       </c>
       <c r="J15" s="92" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K15" s="36" t="s">
         <v>68</v>
@@ -7638,7 +7657,7 @@
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
     </row>
-    <row r="16" spans="1:17" ht="83.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="30">
         <v>9</v>
       </c>
@@ -7661,15 +7680,21 @@
         <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I16" s="92"/>
-      <c r="J16" s="109"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="132" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M16" s="112"/>
+    </row>
+    <row r="17" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="105">
         <v>10</v>
       </c>
@@ -7692,13 +7717,19 @@
         <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I17" s="92"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="132" t="s">
-        <v>198</v>
-      </c>
+      <c r="I17" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="K17" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M17" s="112"/>
     </row>
     <row r="18" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="105">
@@ -7710,7 +7741,7 @@
       <c r="D18" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="E18" s="111" t="s">
+      <c r="E18" s="110" t="s">
         <v>188</v>
       </c>
       <c r="F18" s="32">
@@ -7723,13 +7754,19 @@
         <f>IFERROR(VLOOKUP(G18,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I18" s="92"/>
-      <c r="J18" s="109"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="132" t="s">
-        <v>198</v>
-      </c>
+      <c r="I18" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="109" t="s">
+        <v>200</v>
+      </c>
+      <c r="K18" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="36">
+        <v>42043</v>
+      </c>
+      <c r="M18" s="112"/>
     </row>
     <row r="19" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="105">
@@ -7739,7 +7776,7 @@
         <v>189</v>
       </c>
       <c r="D19" s="104"/>
-      <c r="E19" s="111" t="s">
+      <c r="E19" s="110" t="s">
         <v>190</v>
       </c>
       <c r="F19" s="32">
@@ -7756,7 +7793,7 @@
         <v>57</v>
       </c>
       <c r="J19" s="109" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K19" s="106" t="s">
         <v>68</v>
@@ -7804,6 +7841,7 @@
     <hyperlink ref="D18" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated all test cases
Updated test case and bug metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v1.xlsx
@@ -988,7 +988,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1260,9 +1260,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1305,8 +1302,20 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1361,9 +1370,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1689,7 +1695,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-SG"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1792,8 +1798,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190492000"/>
-        <c:axId val="190492392"/>
+        <c:axId val="340953784"/>
+        <c:axId val="340954176"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2069,11 +2075,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190492000"/>
-        <c:axId val="190492392"/>
+        <c:axId val="340953784"/>
+        <c:axId val="340954176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190492000"/>
+        <c:axId val="340953784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2151,7 +2157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190492392"/>
+        <c:crossAx val="340954176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2159,7 +2165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190492392"/>
+        <c:axId val="340954176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,7 +2202,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190492000"/>
+        <c:crossAx val="340953784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2365,7 +2371,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-SG"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2468,8 +2474,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190493176"/>
-        <c:axId val="190493568"/>
+        <c:axId val="340956528"/>
+        <c:axId val="340956920"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2745,11 +2751,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190493176"/>
-        <c:axId val="190493568"/>
+        <c:axId val="340956528"/>
+        <c:axId val="340956920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190493176"/>
+        <c:axId val="340956528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2827,7 +2833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190493568"/>
+        <c:crossAx val="340956920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2835,7 +2841,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190493568"/>
+        <c:axId val="340956920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190493176"/>
+        <c:crossAx val="340956528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4023,28 +4029,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -4053,30 +4059,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="116" t="s">
+      <c r="G4" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -4647,133 +4653,133 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+    <row r="2" spans="2:6" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="97" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="96">
+      <c r="B3" s="95">
         <v>1</v>
       </c>
-      <c r="C3" s="96">
+      <c r="C3" s="95">
         <v>9</v>
       </c>
-      <c r="D3" s="96">
+      <c r="D3" s="95">
         <v>1</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96">
+      <c r="E3" s="95"/>
+      <c r="F3" s="95">
         <f t="shared" ref="F3:F9" si="0">(C3*1)+(D3*5)+(E3*10)</f>
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="96">
+      <c r="B4" s="95">
         <v>2</v>
       </c>
-      <c r="C4" s="96">
+      <c r="C4" s="95">
         <v>1</v>
       </c>
-      <c r="D4" s="96">
+      <c r="D4" s="95">
         <v>2</v>
       </c>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96">
+      <c r="E4" s="95"/>
+      <c r="F4" s="95">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="96">
+      <c r="B5" s="95">
         <v>3</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96">
+      <c r="C5" s="95"/>
+      <c r="D5" s="95">
         <v>3</v>
       </c>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96">
+      <c r="E5" s="95"/>
+      <c r="F5" s="95">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="96">
+      <c r="B6" s="95">
         <v>4</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96">
+      <c r="C6" s="95"/>
+      <c r="D6" s="95">
         <v>1</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96">
+      <c r="E6" s="95"/>
+      <c r="F6" s="95">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="96">
+      <c r="B7" s="95">
         <v>5</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96">
+      <c r="C7" s="95"/>
+      <c r="D7" s="95">
         <v>6</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96">
+      <c r="E7" s="95"/>
+      <c r="F7" s="95">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="96">
+      <c r="B8" s="95">
         <v>6</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96">
+      <c r="C8" s="95"/>
+      <c r="D8" s="95">
         <v>4</v>
       </c>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96">
+      <c r="E8" s="95"/>
+      <c r="F8" s="95">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="96">
+      <c r="B9" s="95">
         <v>7</v>
       </c>
-      <c r="C9" s="96">
+      <c r="C9" s="95">
         <v>5</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="95">
         <v>3</v>
       </c>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96">
+      <c r="E9" s="95"/>
+      <c r="F9" s="95">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4809,28 +4815,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -4839,30 +4845,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="116" t="s">
+      <c r="G4" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -4971,7 +4977,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
         <v>3</v>
       </c>
@@ -5159,28 +5165,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -5189,30 +5195,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="116" t="s">
+      <c r="G4" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -5510,28 +5516,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="120"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="123"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="122"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -5540,30 +5546,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="123" t="s">
+      <c r="G4" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="128"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="120"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="123"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -5855,28 +5861,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="120"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="123"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="122"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -5885,30 +5891,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="123" t="s">
+      <c r="G4" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="128"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="120"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="123"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -6301,26 +6307,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="128"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="130"/>
+      <c r="C4" s="133"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6329,30 +6335,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="123" t="s">
+      <c r="G4" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="128"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -6713,26 +6719,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="128"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="130"/>
+      <c r="C4" s="133"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6741,30 +6747,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="123" t="s">
+      <c r="G4" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="128"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="78" t="s">
@@ -7213,87 +7219,87 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="43"/>
-    <col min="2" max="2" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="43" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" style="43" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="43" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="43" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="43" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="43" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="43" customWidth="1"/>
-    <col min="10" max="10" width="31" style="43" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="43" customWidth="1"/>
-    <col min="12" max="12" width="14" style="43" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="43" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="1" width="9.140625" style="113"/>
+    <col min="2" max="2" width="4.42578125" style="113" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="113" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="113" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="113" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="113" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="113" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="113" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="113" customWidth="1"/>
+    <col min="10" max="10" width="31" style="113" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="113" customWidth="1"/>
+    <col min="12" max="12" width="14" style="113" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="113" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="128"/>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="129" t="s">
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="131"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="130"/>
+      <c r="C4" s="133"/>
       <c r="D4" s="44">
-        <f>SUM(G8:G116)</f>
+        <f>SUM(G8:G114)</f>
         <v>56</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="123" t="s">
+      <c r="G4" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="125"/>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="126" t="s">
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="128"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="95" t="s">
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="111" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -7302,16 +7308,16 @@
       <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="95" t="s">
+      <c r="E7" s="111" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="95" t="s">
+      <c r="H7" s="111" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -7320,7 +7326,7 @@
       <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="95" t="s">
+      <c r="K7" s="111" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -7331,10 +7337,10 @@
       <c r="B8" s="30">
         <v>1</v>
       </c>
-      <c r="C8" s="102" t="s">
+      <c r="C8" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="103" t="s">
+      <c r="D8" s="102" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="82" t="s">
@@ -7364,14 +7370,14 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="101"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="30">
         <v>2</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="99" t="s">
         <v>168</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -7387,7 +7393,7 @@
         <f>IFERROR(VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
         <v xml:space="preserve">High Impact </v>
       </c>
-      <c r="I9" s="131" t="s">
+      <c r="I9" s="112" t="s">
         <v>57</v>
       </c>
       <c r="J9" s="31" t="s">
@@ -7399,21 +7405,21 @@
       <c r="L9" s="36">
         <v>42043</v>
       </c>
-      <c r="M9" s="111"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="101"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" s="79" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="101"/>
+      <c r="A10" s="100"/>
       <c r="B10" s="30">
         <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="102" t="s">
         <v>172</v>
       </c>
       <c r="E10" s="58" t="s">
@@ -7441,21 +7447,21 @@
       <c r="L10" s="36">
         <v>42043</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="101"/>
-      <c r="Q10" s="101"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
     </row>
     <row r="11" spans="1:17" s="79" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101"/>
+      <c r="A11" s="100"/>
       <c r="B11" s="30">
         <v>4</v>
       </c>
       <c r="C11" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="103" t="s">
         <v>172</v>
       </c>
       <c r="E11" s="58" t="s">
@@ -7483,21 +7489,21 @@
       <c r="L11" s="36">
         <v>42043</v>
       </c>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="101"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="101"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="100"/>
     </row>
     <row r="12" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101"/>
+      <c r="A12" s="100"/>
       <c r="B12" s="30">
         <v>5</v>
       </c>
       <c r="C12" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="103" t="s">
         <v>168</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -7525,11 +7531,11 @@
       <c r="L12" s="36">
         <v>42043</v>
       </c>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="101"/>
-      <c r="P12" s="101"/>
-      <c r="Q12" s="101"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="100"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="100"/>
+      <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="1:17" s="79" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80"/>
@@ -7558,7 +7564,7 @@
       <c r="I13" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="99" t="s">
+      <c r="J13" s="98" t="s">
         <v>198</v>
       </c>
       <c r="K13" s="59" t="s">
@@ -7581,7 +7587,7 @@
       <c r="C14" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="103" t="s">
         <v>180</v>
       </c>
       <c r="E14" s="89" t="s">
@@ -7657,17 +7663,17 @@
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
     </row>
-    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="30">
         <v>9</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="D16" s="108" t="s">
+      <c r="D16" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="E16" s="106" t="s">
+      <c r="E16" s="105" t="s">
         <v>186</v>
       </c>
       <c r="F16" s="32">
@@ -7692,19 +7698,19 @@
       <c r="L16" s="36">
         <v>42043</v>
       </c>
-      <c r="M16" s="112"/>
-    </row>
-    <row r="17" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="105">
+      <c r="M16" s="114"/>
+    </row>
+    <row r="17" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="104">
         <v>10</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="D17" s="104" t="s">
+      <c r="D17" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="106" t="s">
+      <c r="E17" s="105" t="s">
         <v>187</v>
       </c>
       <c r="F17" s="32">
@@ -7729,23 +7735,23 @@
       <c r="L17" s="36">
         <v>42043</v>
       </c>
-      <c r="M17" s="112"/>
-    </row>
-    <row r="18" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="105">
+      <c r="M17" s="114"/>
+    </row>
+    <row r="18" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="104">
         <v>11</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="E18" s="110" t="s">
+      <c r="E18" s="109" t="s">
         <v>188</v>
       </c>
       <c r="F18" s="32">
-        <v>42043</v>
+        <v>42042</v>
       </c>
       <c r="G18" s="92">
         <v>5</v>
@@ -7757,30 +7763,30 @@
       <c r="I18" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="109" t="s">
+      <c r="J18" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="K18" s="106" t="s">
+      <c r="K18" s="105" t="s">
         <v>68</v>
       </c>
       <c r="L18" s="36">
         <v>42043</v>
       </c>
-      <c r="M18" s="112"/>
-    </row>
-    <row r="19" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="105">
+      <c r="M18" s="114"/>
+    </row>
+    <row r="19" spans="2:13" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="104">
         <v>12</v>
       </c>
-      <c r="C19" s="107" t="s">
+      <c r="C19" s="106" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="104"/>
-      <c r="E19" s="110" t="s">
+      <c r="D19" s="103"/>
+      <c r="E19" s="109" t="s">
         <v>190</v>
       </c>
       <c r="F19" s="32">
-        <v>42044</v>
+        <v>42042</v>
       </c>
       <c r="G19" s="92">
         <v>5</v>
@@ -7792,36 +7798,24 @@
       <c r="I19" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="J19" s="109" t="s">
+      <c r="J19" s="108" t="s">
         <v>196</v>
       </c>
-      <c r="K19" s="106" t="s">
+      <c r="K19" s="105" t="s">
         <v>68</v>
       </c>
       <c r="L19" s="36">
         <v>42043</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H20" s="51" t="str">
-        <f>IFERROR(VLOOKUP(G20,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H21" s="51" t="str">
-        <f>IFERROR(VLOOKUP(G21,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H22" s="49"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H23" s="49"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H24" s="49"/>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H20" s="115"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H21" s="115"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H22" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>